<commit_message>
Change AMAU opening hrs
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="10020" windowHeight="5688" tabRatio="914" firstSheet="4" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914" firstSheet="4" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="27" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <definedName name="Values" localSheetId="4">#REF!</definedName>
     <definedName name="Values">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -495,8 +495,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,6 +1073,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1109,8 +1111,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1120,6 +1120,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1166,7 +1174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1198,9 +1206,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,6 +1241,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1407,7 +1417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1417,7 +1427,7 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -1427,24 +1437,24 @@
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="72" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="74" t="s">
+      <c r="D1" s="75"/>
+      <c r="E1" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="75"/>
+      <c r="F1" s="77"/>
       <c r="G1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>64</v>
       </c>
@@ -1468,7 +1478,7 @@
         <v>0.30468505614081465</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>56</v>
       </c>
@@ -1488,7 +1498,7 @@
         <v>40.434618766486622</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>83</v>
       </c>
@@ -1508,7 +1518,7 @@
         <v>66.503391107761871</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>84</v>
       </c>
@@ -1528,7 +1538,7 @@
         <v>7.6577889447236229</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
@@ -1552,7 +1562,7 @@
         <v>0.11317221999602867</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
@@ -1570,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="21" t="s">
         <v>7</v>
       </c>
@@ -1588,7 +1598,7 @@
         <v>5.3706535674163759E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="43" t="s">
         <v>66</v>
       </c>
@@ -1608,7 +1618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1618,23 +1628,23 @@
       <selection activeCell="D9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="71"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="C1" s="83"/>
+      <c r="D1" s="73"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>50</v>
       </c>
@@ -1648,7 +1658,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
@@ -1662,7 +1672,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>52</v>
       </c>
@@ -1676,13 +1686,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="62"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>58</v>
       </c>
@@ -1705,19 +1715,19 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>59</v>
       </c>
@@ -1740,7 +1750,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>60</v>
       </c>
@@ -1754,7 +1764,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>61</v>
       </c>
@@ -1768,7 +1778,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>62</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>108</v>
       </c>
@@ -1812,7 +1822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1820,23 +1830,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="71"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="C1" s="83"/>
+      <c r="D1" s="73"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>63</v>
       </c>
@@ -1850,7 +1860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>64</v>
       </c>
@@ -1864,7 +1874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>65</v>
       </c>
@@ -1878,7 +1888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
         <v>111</v>
       </c>
@@ -1892,7 +1902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="57" t="s">
         <v>112</v>
       </c>
@@ -1906,7 +1916,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="58" t="s">
         <v>113</v>
       </c>
@@ -1920,7 +1930,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="58" t="s">
         <v>114</v>
       </c>
@@ -1934,7 +1944,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="58" t="s">
         <v>115</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>109</v>
       </c>
@@ -1969,7 +1979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1979,12 +1989,12 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>86</v>
       </c>
@@ -1992,7 +2002,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2014,7 +2024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -2050,7 +2060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -2061,7 +2071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2082,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -2083,7 +2093,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2097,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -2108,7 +2118,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2119,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>113</v>
       </c>
@@ -2130,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>114</v>
       </c>
@@ -2141,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>81</v>
       </c>
@@ -2152,7 +2162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>112</v>
       </c>
@@ -2163,7 +2173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>116</v>
       </c>
@@ -2174,7 +2184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>88</v>
       </c>
@@ -2185,7 +2195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>115</v>
       </c>
@@ -2203,7 +2213,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2211,12 +2221,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>86</v>
       </c>
@@ -2224,7 +2234,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2235,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2246,7 +2256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2268,7 +2278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -2293,7 +2303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2304,7 +2314,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -2315,7 +2325,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2329,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -2340,7 +2350,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2351,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>113</v>
       </c>
@@ -2362,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>114</v>
       </c>
@@ -2373,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>81</v>
       </c>
@@ -2384,7 +2394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>112</v>
       </c>
@@ -2395,7 +2405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>116</v>
       </c>
@@ -2406,7 +2416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>88</v>
       </c>
@@ -2417,7 +2427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>115</v>
       </c>
@@ -2435,7 +2445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2443,13 +2453,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2482,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
@@ -2493,7 +2503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2516,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -2562,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -2585,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -2631,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>8</v>
       </c>
@@ -2652,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -2675,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -2698,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -2719,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>118</v>
       </c>
@@ -2742,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>119</v>
       </c>
@@ -2765,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>120</v>
       </c>
@@ -2788,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>121</v>
       </c>
@@ -2818,7 +2828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2826,7 +2836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -2837,7 +2847,7 @@
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -2860,7 +2870,7 @@
       </c>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -2882,7 +2892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -2905,7 +2915,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -2928,7 +2938,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -2947,7 +2957,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -2966,7 +2976,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -2980,7 +2990,7 @@
       </c>
       <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -2994,7 +3004,7 @@
       </c>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -3008,7 +3018,7 @@
       </c>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -3022,7 +3032,7 @@
       </c>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -3036,7 +3046,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -3050,7 +3060,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -3064,7 +3074,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -3078,7 +3088,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -3092,7 +3102,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -3106,7 +3116,7 @@
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -3120,7 +3130,7 @@
       </c>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -3134,7 +3144,7 @@
       </c>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -3148,7 +3158,7 @@
       </c>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -3162,7 +3172,7 @@
       </c>
       <c r="H20" s="25"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -3176,7 +3186,7 @@
       </c>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -3190,7 +3200,7 @@
       </c>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -3204,7 +3214,7 @@
       </c>
       <c r="H23" s="25"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -3234,7 +3244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -3242,13 +3252,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -3257,7 +3267,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -3269,7 +3279,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -3289,7 +3299,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -3312,7 +3322,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -3336,7 +3346,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -3360,7 +3370,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -3374,103 +3384,103 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
       <c r="B8" s="25"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
       <c r="B9" s="25"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
       <c r="B10" s="25"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
       <c r="B11" s="25"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
       <c r="B12" s="25"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
       <c r="B13" s="25"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
       <c r="B14" s="25"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
       <c r="B15" s="25"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
       <c r="B16" s="25"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
       <c r="B17" s="25"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
       <c r="B19" s="25"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
       <c r="B20" s="25"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
       <c r="B21" s="25"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
       <c r="B22" s="25"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
       <c r="B23" s="25"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -3485,14 +3495,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -3504,7 +3514,7 @@
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -3525,7 +3535,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -3546,7 +3556,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -3592,7 +3602,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -3611,7 +3621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -3630,7 +3640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -3645,7 +3655,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -3659,7 +3669,7 @@
       </c>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -3673,7 +3683,7 @@
       </c>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -3687,7 +3697,7 @@
       </c>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -3701,7 +3711,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -3715,7 +3725,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -3729,7 +3739,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -3743,7 +3753,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -3757,7 +3767,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -3771,7 +3781,7 @@
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -3785,7 +3795,7 @@
       </c>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -3799,7 +3809,7 @@
       </c>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -3813,7 +3823,7 @@
       </c>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -3827,7 +3837,7 @@
       </c>
       <c r="H20" s="25"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -3841,7 +3851,7 @@
       </c>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -3855,7 +3865,7 @@
       </c>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -3869,7 +3879,7 @@
       </c>
       <c r="H23" s="25"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -3899,7 +3909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -3908,7 +3918,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.109375" style="26" bestFit="1" customWidth="1"/>
@@ -3918,7 +3928,7 @@
     <col min="9" max="9" width="20.33203125" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -3938,7 +3948,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -3958,7 +3968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -3978,7 +3988,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -3998,7 +4008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -4016,7 +4026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -4030,7 +4040,7 @@
       </c>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -4044,7 +4054,7 @@
       </c>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -4058,7 +4068,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -4072,7 +4082,7 @@
       </c>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -4086,7 +4096,7 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -4100,7 +4110,7 @@
       </c>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -4114,7 +4124,7 @@
       </c>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -4128,7 +4138,7 @@
       </c>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -4142,7 +4152,7 @@
       </c>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -4156,7 +4166,7 @@
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -4170,7 +4180,7 @@
       </c>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -4184,7 +4194,7 @@
       </c>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -4198,7 +4208,7 @@
       </c>
       <c r="I18" s="25"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -4212,7 +4222,7 @@
       </c>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -4226,7 +4236,7 @@
       </c>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -4240,7 +4250,7 @@
       </c>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -4254,7 +4264,7 @@
       </c>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -4268,7 +4278,7 @@
       </c>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -4298,7 +4308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4308,7 +4318,7 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.109375" style="26" bestFit="1" customWidth="1"/>
@@ -4322,7 +4332,7 @@
     <col min="14" max="14" width="20.33203125" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -4354,7 +4364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -4386,7 +4396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -4423,7 +4433,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -4460,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -4497,7 +4507,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -4534,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -4571,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -4608,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -4645,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -4682,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -4719,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -4756,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -4793,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -4830,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -4867,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -4904,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -4941,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -4978,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -5015,7 +5025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -5052,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -5089,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -5126,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -5163,7 +5173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -5207,7 +5217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -5217,14 +5227,14 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -5234,7 +5244,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
@@ -5245,7 +5255,7 @@
     <col min="9" max="9" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -5269,7 +5279,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -5293,7 +5303,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -5319,7 +5329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -5345,7 +5355,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -5369,7 +5379,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -5388,7 +5398,7 @@
       </c>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -5402,7 +5412,7 @@
       </c>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -5416,7 +5426,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -5430,7 +5440,7 @@
       </c>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -5444,7 +5454,7 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -5458,7 +5468,7 @@
       </c>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -5472,7 +5482,7 @@
       </c>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -5486,7 +5496,7 @@
       </c>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -5500,7 +5510,7 @@
       </c>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -5514,7 +5524,7 @@
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -5528,7 +5538,7 @@
       </c>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -5542,7 +5552,7 @@
       </c>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -5556,7 +5566,7 @@
       </c>
       <c r="I18" s="25"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -5570,7 +5580,7 @@
       </c>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -5584,7 +5594,7 @@
       </c>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -5598,7 +5608,7 @@
       </c>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -5612,7 +5622,7 @@
       </c>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -5626,7 +5636,7 @@
       </c>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -5655,14 +5665,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
@@ -5674,7 +5684,7 @@
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -5704,7 +5714,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -5734,7 +5744,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -5764,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -5794,7 +5804,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -5824,7 +5834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -5854,7 +5864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -5884,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -5914,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -5944,7 +5954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -5974,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -6004,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -6034,7 +6044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -6064,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -6094,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -6124,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -6154,7 +6164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -6184,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -6214,7 +6224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -6244,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -6274,7 +6284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -6304,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -6334,7 +6344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -6364,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -6400,7 +6410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -6410,7 +6420,7 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
@@ -6419,7 +6429,7 @@
     <col min="7" max="7" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -6436,7 +6446,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -6453,7 +6463,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -6467,7 +6477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -6481,7 +6491,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -6493,7 +6503,7 @@
       </c>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -6505,7 +6515,7 @@
       </c>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -6515,7 +6525,7 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -6525,7 +6535,7 @@
       </c>
       <c r="F8" s="25"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -6535,7 +6545,7 @@
       </c>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -6545,7 +6555,7 @@
       </c>
       <c r="F10" s="25"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -6555,7 +6565,7 @@
       </c>
       <c r="F11" s="25"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -6565,7 +6575,7 @@
       </c>
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -6575,7 +6585,7 @@
       </c>
       <c r="F13" s="25"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -6585,7 +6595,7 @@
       </c>
       <c r="F14" s="25"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -6595,7 +6605,7 @@
       </c>
       <c r="F15" s="25"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -6605,7 +6615,7 @@
       </c>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -6615,7 +6625,7 @@
       </c>
       <c r="F17" s="25"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -6625,7 +6635,7 @@
       </c>
       <c r="F18" s="25"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -6635,7 +6645,7 @@
       </c>
       <c r="F19" s="25"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -6645,7 +6655,7 @@
       </c>
       <c r="F20" s="25"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -6655,7 +6665,7 @@
       </c>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -6665,7 +6675,7 @@
       </c>
       <c r="F22" s="25"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -6675,7 +6685,7 @@
       </c>
       <c r="F23" s="25"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -6697,14 +6707,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
@@ -6717,7 +6727,7 @@
     <col min="12" max="12" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -6747,7 +6757,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -6777,7 +6787,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -6807,7 +6817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -6837,7 +6847,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -6867,7 +6877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -6897,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -6927,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -6957,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -6987,7 +6997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -7017,7 +7027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -7047,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -7077,7 +7087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -7107,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -7137,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -7167,7 +7177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -7197,7 +7207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -7227,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -7257,7 +7267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -7287,7 +7297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -7317,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -7347,7 +7357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -7377,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -7407,7 +7417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -7443,7 +7453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -7453,7 +7463,7 @@
       <selection activeCell="I3" sqref="I3:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
@@ -7464,7 +7474,7 @@
     <col min="9" max="9" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -7488,7 +7498,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -7512,7 +7522,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -7538,7 +7548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -7564,7 +7574,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -7588,7 +7598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -7607,7 +7617,7 @@
       </c>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -7621,7 +7631,7 @@
       </c>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -7635,7 +7645,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -7649,7 +7659,7 @@
       </c>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -7663,7 +7673,7 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -7677,7 +7687,7 @@
       </c>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -7691,7 +7701,7 @@
       </c>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -7705,7 +7715,7 @@
       </c>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -7719,7 +7729,7 @@
       </c>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -7733,7 +7743,7 @@
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -7747,7 +7757,7 @@
       </c>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -7761,7 +7771,7 @@
       </c>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -7775,7 +7785,7 @@
       </c>
       <c r="I18" s="25"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -7789,7 +7799,7 @@
       </c>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -7803,7 +7813,7 @@
       </c>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -7817,7 +7827,7 @@
       </c>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -7831,7 +7841,7 @@
       </c>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -7845,7 +7855,7 @@
       </c>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -7874,7 +7884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -7884,7 +7894,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
@@ -7892,7 +7902,7 @@
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -7907,7 +7917,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -7922,7 +7932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -7939,7 +7949,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -7956,7 +7966,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -7971,7 +7981,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -7986,7 +7996,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -8001,7 +8011,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -8016,7 +8026,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -8026,7 +8036,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -8036,7 +8046,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -8046,7 +8056,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -8056,7 +8066,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -8066,7 +8076,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -8076,7 +8086,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -8086,7 +8096,7 @@
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -8096,7 +8106,7 @@
       </c>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -8106,7 +8116,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -8116,7 +8126,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -8126,7 +8136,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -8136,7 +8146,7 @@
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -8146,7 +8156,7 @@
       </c>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -8156,7 +8166,7 @@
       </c>
       <c r="E22" s="25"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -8166,7 +8176,7 @@
       </c>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -8188,12 +8198,12 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -8205,7 +8215,7 @@
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" s="64" customFormat="1">
+    <row r="1" spans="2:24" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
         <v>7.3124413473795506</v>
       </c>
@@ -8267,7 +8277,7 @@
         <v>2.3005384238864415E-2</v>
       </c>
     </row>
-    <row r="2" spans="2:24">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="68">
         <v>24.11969675609075</v>
       </c>
@@ -8329,7 +8339,7 @@
         <v>2.7587472473697087E-2</v>
       </c>
     </row>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B3" s="68">
         <v>21.91588362706678</v>
       </c>
@@ -8391,7 +8401,7 @@
         <v>2.7010695510302739E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:24">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" s="68">
         <v>14.651612248687435</v>
       </c>
@@ -8453,7 +8463,7 @@
         <v>2.9150138237768963E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:24">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" s="68">
         <v>15.639982038500012</v>
       </c>
@@ -8515,7 +8525,7 @@
         <v>2.6551913568943417E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:24">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
       <c r="D6" s="68"/>
@@ -8527,7 +8537,7 @@
       <c r="J6" s="68"/>
       <c r="K6" s="68"/>
     </row>
-    <row r="7" spans="2:24">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" s="68"/>
       <c r="C7" s="68"/>
       <c r="D7" s="68"/>
@@ -8539,7 +8549,7 @@
       <c r="J7" s="68"/>
       <c r="K7" s="68"/>
     </row>
-    <row r="8" spans="2:24">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -8551,7 +8561,7 @@
       <c r="J8" s="68"/>
       <c r="K8" s="68"/>
     </row>
-    <row r="9" spans="2:24">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
@@ -8563,7 +8573,7 @@
       <c r="J9" s="68"/>
       <c r="K9" s="68"/>
     </row>
-    <row r="10" spans="2:24">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="68"/>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
@@ -8575,7 +8585,7 @@
       <c r="J10" s="68"/>
       <c r="K10" s="68"/>
     </row>
-    <row r="11" spans="2:24">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B11" s="66"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
@@ -8587,7 +8597,7 @@
       <c r="J11" s="66"/>
       <c r="K11" s="66"/>
     </row>
-    <row r="12" spans="2:24">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
@@ -8599,7 +8609,7 @@
       <c r="J12" s="66"/>
       <c r="K12" s="66"/>
     </row>
-    <row r="13" spans="2:24">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B5)</f>
         <v>16.727923203544904</v>
@@ -8681,7 +8691,7 @@
         <v>2.6661120805915327E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="15.6">
+    <row r="16" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="63" t="s">
         <v>124</v>
       </c>
@@ -8713,36 +8723,36 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1"/>
-    <row r="18" spans="2:11" s="82" customFormat="1">
-      <c r="B18" s="82">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:11" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="70">
         <v>10</v>
       </c>
-      <c r="C18" s="82">
+      <c r="C18" s="70">
         <v>16</v>
       </c>
-      <c r="D18" s="82">
+      <c r="D18" s="70">
         <v>6.7</v>
       </c>
-      <c r="E18" s="83">
+      <c r="E18" s="71">
         <v>0.32020999999999999</v>
       </c>
-      <c r="F18" s="83">
+      <c r="F18" s="71">
         <v>0.56228999999999996</v>
       </c>
-      <c r="G18" s="83">
+      <c r="G18" s="71">
         <v>0.47022000000000003</v>
       </c>
-      <c r="H18" s="83">
+      <c r="H18" s="71">
         <v>0.77647999999999995</v>
       </c>
-      <c r="I18" s="83">
+      <c r="I18" s="71">
         <v>0.89500000000000002</v>
       </c>
-      <c r="J18" s="83">
+      <c r="J18" s="71">
         <v>0.38</v>
       </c>
-      <c r="K18" s="82">
+      <c r="K18" s="70">
         <v>0.1</v>
       </c>
     </row>
@@ -8753,7 +8763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -8761,7 +8771,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -8774,7 +8784,7 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="str">
         <f>Resus!A1</f>
         <v>Resources/Process</v>
@@ -8816,7 +8826,7 @@
         <v>Clean</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="str">
         <f>Resus!A2</f>
         <v>Time</v>
@@ -8858,7 +8868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1">
+    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>Resus!A3</f>
         <v>Consultant</v>
@@ -8900,7 +8910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1">
+    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>Resus!A4</f>
         <v>Registrar</v>
@@ -8942,7 +8952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="4" customFormat="1">
+    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>Resus!A5</f>
         <v>SHO</v>
@@ -8984,7 +8994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="4" customFormat="1">
+    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>Resus!A6</f>
         <v>Nurses</v>
@@ -9026,7 +9036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="4" customFormat="1">
+    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>Resus!A7</f>
         <v>Porters</v>
@@ -9068,7 +9078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1">
+    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>Resus!A8</f>
         <v>Cleaners</v>
@@ -9110,7 +9120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1">
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="str">
         <f>Resus!A9</f>
         <v>Trolly</v>
@@ -9152,7 +9162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1">
+    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f>Resus!A10</f>
         <v>Wheelchair</v>
@@ -9194,7 +9204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1">
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f>Resus!A11</f>
         <v>Portable Xray</v>
@@ -9236,7 +9246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1">
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="str">
         <f>Resus!A12</f>
         <v>Cubicle</v>
@@ -9278,10 +9288,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="str">
         <f>Resus!A14</f>
         <v>Zone Capacity:</v>
@@ -9298,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -9306,7 +9316,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -9319,7 +9329,7 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -9351,7 +9361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
@@ -9383,7 +9393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1">
+    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -9415,7 +9425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1">
+    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -9447,7 +9457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="4" customFormat="1">
+    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -9479,7 +9489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="4" customFormat="1">
+    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -9511,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="4" customFormat="1">
+    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -9543,7 +9553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1">
+    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -9575,7 +9585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1">
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>8</v>
       </c>
@@ -9607,7 +9617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1">
+    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -9639,7 +9649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1">
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -9671,7 +9681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1">
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -9703,10 +9713,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -9714,7 +9724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
@@ -9746,8 +9756,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="76" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="78" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -9781,8 +9791,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="77"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="79"/>
       <c r="B20" s="8">
         <v>2</v>
       </c>
@@ -9814,8 +9824,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="77"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="79"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -9857,7 +9867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -9867,7 +9877,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -9882,7 +9892,7 @@
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -9912,7 +9922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
@@ -9942,7 +9952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -9972,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -10002,7 +10012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -10032,7 +10042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -10062,7 +10072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -10092,7 +10102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -10122,7 +10132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>8</v>
       </c>
@@ -10152,7 +10162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -10182,7 +10192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -10212,7 +10222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -10242,10 +10252,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -10253,7 +10263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
@@ -10261,7 +10271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
@@ -10294,8 +10304,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="80" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -10330,8 +10340,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="81"/>
       <c r="B20" s="8">
         <v>7</v>
       </c>
@@ -10364,8 +10374,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="80"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="82"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -10408,7 +10418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -10416,7 +10426,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -10429,7 +10439,7 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -10459,7 +10469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -10497,7 +10507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -10535,7 +10545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -10573,7 +10583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -10611,7 +10621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -10649,7 +10659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -10687,7 +10697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -10725,7 +10735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
@@ -10755,7 +10765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -10793,7 +10803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -10831,7 +10841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>12</v>
       </c>
@@ -10861,10 +10871,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -10873,7 +10883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
@@ -10889,7 +10899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -10899,7 +10909,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -10914,7 +10924,7 @@
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -10944,7 +10954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
@@ -10974,7 +10984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -11004,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -11034,7 +11044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -11064,7 +11074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -11094,7 +11104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -11124,7 +11134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -11154,7 +11164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>8</v>
       </c>
@@ -11184,7 +11194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -11214,7 +11224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -11244,7 +11254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -11274,10 +11284,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -11285,7 +11295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
@@ -11293,7 +11303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
@@ -11326,8 +11336,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="80" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -11362,8 +11372,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="81"/>
       <c r="B20" s="8">
         <v>7</v>
       </c>
@@ -11396,8 +11406,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="80"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="82"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -11440,7 +11450,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -11449,7 +11459,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -11462,7 +11472,7 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -11492,7 +11502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
@@ -11522,7 +11532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -11552,7 +11562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -11582,7 +11592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -11612,7 +11622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -11642,7 +11652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -11672,7 +11682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -11702,7 +11712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>8</v>
       </c>
@@ -11732,7 +11742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -11762,7 +11772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -11792,7 +11802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -11822,10 +11832,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -11836,11 +11846,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
@@ -11870,7 +11880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
         <v>1</v>
       </c>
@@ -11903,7 +11913,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="52"/>
       <c r="B20" s="8">
         <v>2</v>
@@ -11934,7 +11944,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
       <c r="B21" s="8">
         <v>1</v>
@@ -11972,7 +11982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -11982,7 +11992,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -11995,7 +12005,7 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="str">
         <f>Minor!A1</f>
         <v>Resources/Process</v>
@@ -12037,7 +12047,7 @@
         <v>Clean</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="str">
         <f>Minor!A2</f>
         <v>Time</v>
@@ -12079,7 +12089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -12120,7 +12130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -12161,7 +12171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -12202,7 +12212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -12243,7 +12253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -12284,7 +12294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -12325,7 +12335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
@@ -12358,7 +12368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -12399,7 +12409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -12440,7 +12450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>12</v>
       </c>
@@ -12473,10 +12483,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -12488,7 +12498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update layout + waiting spaces for mjrs
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914" firstSheet="4" activeTab="25"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="27" r:id="rId1"/>
@@ -1423,8 +1423,8 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,23 +1459,23 @@
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16664044059795421</v>
+        <v>0.16665315059605881</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>0.32505006766681138</v>
+        <v>0.30223817384103313</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>438.74648084277305</v>
+        <v>3928.3779089905652</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>0.30468505614081465</v>
+        <v>2.7280402145767813</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1489,13 +1489,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.28719377069695268</v>
+        <v>0.64009434942150867</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>40.434618766486622</v>
+        <v>19.741817707654192</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1503,19 +1503,19 @@
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>0.50959095528455245</v>
+        <v>5.973502457165619</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>1.1133841242085751E-2</v>
+        <v>2.7244130262917644E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>66.503391107761871</v>
+        <v>28.254775409087944</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1523,19 +1523,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>0.44923995864762423</v>
+        <v>-0.58021149848072884</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>0.24220783152004319</v>
+        <v>0.53022380538046221</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.6577889447236229</v>
+        <v>7.6513326499231269</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1543,23 +1543,23 @@
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>8.9509888220120418E-2</v>
+        <v>0.14406256884776439</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.10519610156380195</v>
+        <v>0.20224736216484754</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>162.96799679428128</v>
+        <v>474.28252271116156</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>0.11317221999602867</v>
+        <v>0.32936286299386219</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1567,7 +1567,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.196523811720205</v>
+        <v>0.44078819178150652</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -1585,17 +1585,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>3.9984040215546322E-2</v>
+        <v>8.9662625880046573E-2</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>7.7337411370795818E-3</v>
+        <v>1.1093633415294735</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>5.3706535674163759E-6</v>
+        <v>7.703912093954677E-4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2189,7 +2189,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="12">
         <v>7</v>
@@ -8201,7 +8201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8217,34 +8217,34 @@
   <sheetData>
     <row r="1" spans="2:24" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>7.3124413473795506</v>
+        <v>65.47296514984275</v>
       </c>
       <c r="C1" s="68">
-        <v>10.134311276161366</v>
+        <v>133.88060461473657</v>
       </c>
       <c r="D1" s="68">
-        <v>4.4948254938672694</v>
+        <v>8.3109781017719193</v>
       </c>
       <c r="E1" s="68">
-        <v>40.404675128817388</v>
+        <v>19.746967523151167</v>
       </c>
       <c r="F1" s="68">
-        <v>66.486554410655941</v>
+        <v>28.262145418976196</v>
       </c>
       <c r="G1" s="68">
-        <v>72.934973637961335</v>
+        <v>36.193895870736085</v>
       </c>
       <c r="H1" s="68">
-        <v>92.570281124497996</v>
+        <v>51.591670655816181</v>
       </c>
       <c r="I1" s="68">
-        <v>0.93000709387562075</v>
+        <v>0.89280918080820415</v>
       </c>
       <c r="J1" s="68">
-        <v>0.49290612437928588</v>
+        <v>0.44994506165303383</v>
       </c>
       <c r="K1" s="68">
-        <v>2.1754551903523291E-2</v>
+        <v>5.7563179099011111E-2</v>
       </c>
       <c r="O1" s="68">
         <v>9.3255076414271194</v>
@@ -8612,43 +8612,43 @@
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B5)</f>
-        <v>16.727923203544904</v>
+        <v>28.360027964037545</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:K13" si="0">AVERAGE(C1:C5)</f>
-        <v>27.690478592555309</v>
+        <v>52.439737260270348</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>6.4436032482055765</v>
+        <v>7.2068337697865079</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>27.467148256358588</v>
+        <v>23.335606735225344</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>43.291530069377693</v>
+        <v>35.646648271041741</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>51.890176162588418</v>
+        <v>44.541960609143381</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>74.706815995399126</v>
+        <v>66.511093901662775</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.92928286031926322</v>
+        <v>0.92184327770577978</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.49222541908403805</v>
+        <v>0.48363320653878761</v>
       </c>
       <c r="K13" s="67">
         <f t="shared" si="0"/>
-        <v>2.8852637134338804E-2</v>
+        <v>3.6014362573436362E-2</v>
       </c>
       <c r="O13" s="67">
         <f>AVERAGE(O1:O5)</f>

</xml_diff>

<commit_message>
Update interarrival to include AMAU + dist % of categories
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="27" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="142">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -490,12 +490,18 @@
   </si>
   <si>
     <t>AMAU_2_SSU_discharge_admit</t>
+  </si>
+  <si>
+    <t>From Data of ED + AMAU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -920,7 +926,7 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1111,6 +1117,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1459,23 +1466,23 @@
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16665315059605881</v>
+        <v>0.16666162609002497</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>0.30223817384103313</v>
+        <v>10.978841897973325</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>3928.3779089905652</v>
+        <v>572.30647262032824</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>2.7280402145767813</v>
+        <v>0.39743505043078348</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1489,13 +1496,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.64009434942150867</v>
+        <v>0.77403013118876773</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>19.741817707654192</v>
+        <v>32.286758342148289</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1503,19 +1510,19 @@
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>5.973502457165619</v>
+        <v>1.3526256490643651</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>2.7244130262917644E-2</v>
+        <v>8.9675200192274152E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>28.254775409087944</v>
+        <v>51.098610510120679</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1523,19 +1530,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>-0.58021149848072884</v>
+        <v>-0.23332211909520939</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>0.53022380538046221</v>
+        <v>0.65344681025284346</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.6513326499231269</v>
+        <v>7.6490997749437373</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1543,23 +1550,23 @@
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>0.14406256884776439</v>
+        <v>0.33739289386496057</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.20224736216484754</v>
+        <v>0.27240387557548817</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>474.28252271116156</v>
+        <v>192.04148267250656</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>0.32936286299386219</v>
+        <v>0.13336214074479621</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1567,7 +1574,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.44078819178150652</v>
+        <v>0.11750510529954228</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -1585,17 +1592,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>8.9662625880046573E-2</v>
+        <v>0.11204107703115605</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>1.1093633415294735</v>
+        <v>25.557435173782309</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>7.703912093954677E-4</v>
+        <v>1.7748218870682158E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1986,7 +1993,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2189,7 +2196,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="12">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D18" s="12">
         <v>7</v>
@@ -3248,9 +3255,11 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3258,7 +3267,7 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -3267,7 +3276,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -3278,13 +3287,16 @@
       <c r="H2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
       <c r="B3" s="25">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="C3" t="s">
         <v>134</v>
@@ -3298,13 +3310,16 @@
       <c r="H3" s="25">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="84">
+        <v>7.9047792113392697E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
       <c r="B4" s="25">
-        <v>25.8</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="C4" t="s">
         <v>135</v>
@@ -3321,14 +3336,16 @@
       <c r="H4" s="25">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="84">
+        <v>0.18408141013992368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
       <c r="B5" s="25">
-        <f>55.5</f>
-        <v>55.5</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>136</v>
@@ -3345,14 +3362,16 @@
       <c r="H5" s="25">
         <v>55.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="84">
+        <v>0.50999454842813008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
       <c r="B6" s="25">
-        <f>15.2</f>
-        <v>15.2</v>
+        <v>24.8</v>
       </c>
       <c r="C6" t="s">
         <v>137</v>
@@ -3369,13 +3388,16 @@
       <c r="H6" s="25">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="84">
+        <v>0.2476376521897147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
       <c r="B7" s="25">
-        <v>2.1</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>138</v>
@@ -3383,56 +3405,59 @@
       <c r="H7" s="25">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="84">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
       <c r="B8" s="25"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
       <c r="B9" s="25"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
       <c r="B10" s="25"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
       <c r="B11" s="25"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
       <c r="B12" s="25"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
       <c r="B13" s="25"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
       <c r="B14" s="25"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
       <c r="B15" s="25"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -8217,34 +8242,34 @@
   <sheetData>
     <row r="1" spans="2:24" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>65.47296514984275</v>
+        <v>9.5384412103388048</v>
       </c>
       <c r="C1" s="68">
-        <v>133.88060461473657</v>
+        <v>13.152080289277446</v>
       </c>
       <c r="D1" s="68">
-        <v>8.3109781017719193</v>
+        <v>6.6752552815003963</v>
       </c>
       <c r="E1" s="68">
-        <v>19.746967523151167</v>
+        <v>32.27373280754064</v>
       </c>
       <c r="F1" s="68">
-        <v>28.262145418976196</v>
+        <v>51.089204135609521</v>
       </c>
       <c r="G1" s="68">
-        <v>36.193895870736085</v>
+        <v>55.925191760751524</v>
       </c>
       <c r="H1" s="68">
-        <v>51.591670655816181</v>
+        <v>74.982764563943476</v>
       </c>
       <c r="I1" s="68">
-        <v>0.89280918080820415</v>
+        <v>0.89569882695280534</v>
       </c>
       <c r="J1" s="68">
-        <v>0.44994506165303383</v>
+        <v>0.44162044193871058</v>
       </c>
       <c r="K1" s="68">
-        <v>5.7563179099011111E-2</v>
+        <v>6.4335727925797948E-2</v>
       </c>
       <c r="O1" s="68">
         <v>9.3255076414271194</v>
@@ -8612,43 +8637,43 @@
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B5)</f>
-        <v>28.360027964037545</v>
+        <v>17.173123176136759</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:K13" si="0">AVERAGE(C1:C5)</f>
-        <v>52.439737260270348</v>
+        <v>28.294032395178522</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>7.2068337697865079</v>
+        <v>6.8796892057322028</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>23.335606735225344</v>
+        <v>25.840959792103241</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>35.646648271041741</v>
+        <v>40.212060014368411</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>44.541960609143381</v>
+        <v>48.488219787146463</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>66.511093901662775</v>
+        <v>71.189312683288236</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.92184327770577978</v>
+        <v>0.92242120693470009</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.48363320653878761</v>
+        <v>0.48196828259592295</v>
       </c>
       <c r="K13" s="67">
         <f t="shared" si="0"/>
-        <v>3.6014362573436362E-2</v>
+        <v>3.7368872338793734E-2</v>
       </c>
       <c r="O13" s="67">
         <f>AVERAGE(O1:O5)</f>

</xml_diff>

<commit_message>
Changes include change of resources, inter-arrival rates, percentages of cat... etc
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="27" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +656,13 @@
       <color theme="0"/>
       <name val="Constantia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="23">
@@ -920,13 +927,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1081,6 +1089,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1117,13 +1126,14 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1430,8 +1440,8 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1445,18 +1455,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="76" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="77"/>
+      <c r="F1" s="78"/>
       <c r="G1" t="s">
         <v>122</v>
       </c>
@@ -1466,23 +1476,23 @@
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16666162609002497</v>
+        <v>0.16665809988863167</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>10.978841897973325</v>
+        <v>0</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>572.30647262032824</v>
+        <v>522.71862571155793</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>0.39743505043078348</v>
+        <v>0.36299904563302632</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1496,13 +1506,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.77403013118876773</v>
+        <v>0.31359020559469553</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>32.286758342148289</v>
+        <v>35.78078713499788</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1510,19 +1520,19 @@
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>1.3526256490643651</v>
+        <v>0.17403314917127075</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>8.9675200192274152E-2</v>
+        <v>1.5443285402759037E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>51.098610510120679</v>
+        <v>58.320110017983708</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1530,19 +1540,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>-0.23332211909520939</v>
+        <v>0.52326906667143624</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>0.65344681025284346</v>
+        <v>0.41193920111787602</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.6490997749437373</v>
+        <v>7.474015226746106</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1550,23 +1560,23 @@
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>0.33739289386496057</v>
+        <v>0.12325084020776028</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.27240387557548817</v>
+        <v>8.6391768177902645E-2</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>192.04148267250656</v>
+        <v>154.82842161969543</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>0.13336214074479621</v>
+        <v>0.10751973723589961</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1574,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.11750510529954228</v>
+        <v>0.41126947967374333</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -1592,17 +1602,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>0.11204107703115605</v>
+        <v>0.15704874392181789</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>25.557435173782309</v>
+        <v>1.7683926345987855</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>1.7748218870682158E-2</v>
+        <v>1.228050440693601E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1631,9 +1641,7 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="B9:D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1645,11 +1653,11 @@
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="73"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
@@ -1835,7 +1843,9 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1847,11 +1857,11 @@
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="73"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -1864,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="30">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,13 +1896,13 @@
         <v>65</v>
       </c>
       <c r="B4" s="30">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C4" s="30">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" s="30">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1906,7 +1916,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="30">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,13 +1924,13 @@
         <v>112</v>
       </c>
       <c r="B6" s="30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C6" s="30">
         <v>10</v>
       </c>
       <c r="D6" s="30">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,13 +1938,13 @@
         <v>113</v>
       </c>
       <c r="B7" s="30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C7" s="30">
         <v>10</v>
       </c>
       <c r="D7" s="30">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,13 +1952,13 @@
         <v>114</v>
       </c>
       <c r="B8" s="30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C8" s="30">
         <v>10</v>
       </c>
       <c r="D8" s="30">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,13 +1966,13 @@
         <v>115</v>
       </c>
       <c r="B9" s="30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C9" s="30">
         <v>10</v>
       </c>
       <c r="D9" s="30">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1993,7 +2003,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2057,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="12">
         <v>11</v>
@@ -2058,7 +2068,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2072,7 +2082,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
@@ -2083,7 +2093,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="12">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D8" s="12">
         <v>36</v>
@@ -2130,7 +2140,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
@@ -2174,7 +2184,7 @@
         <v>112</v>
       </c>
       <c r="B16" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16" s="12">
         <v>3</v>
@@ -2196,7 +2206,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="12">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D18" s="12">
         <v>7</v>
@@ -2226,7 +2236,9 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2268,7 +2280,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="12">
         <v>10</v>
@@ -2279,7 +2291,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="12">
         <v>11</v>
@@ -2841,7 +2853,9 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2904,6 +2918,9 @@
         <v>0</v>
       </c>
       <c r="B3" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="C3">
         <v>25</v>
       </c>
       <c r="D3" s="22">
@@ -2927,6 +2944,9 @@
         <v>1</v>
       </c>
       <c r="B4" s="25">
+        <v>98.75</v>
+      </c>
+      <c r="C4">
         <v>75</v>
       </c>
       <c r="D4" s="22">
@@ -3257,9 +3277,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3296,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="25">
-        <v>0.8</v>
+        <v>1.3</v>
       </c>
       <c r="C3" t="s">
         <v>134</v>
@@ -3310,8 +3328,8 @@
       <c r="H3" s="25">
         <v>1.4</v>
       </c>
-      <c r="I3" s="84">
-        <v>7.9047792113392697E-3</v>
+      <c r="I3" s="72">
+        <v>1.250882679309997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3319,7 +3337,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="25">
-        <v>18.399999999999999</v>
+        <v>25.9</v>
       </c>
       <c r="C4" t="s">
         <v>135</v>
@@ -3336,8 +3354,8 @@
       <c r="H4" s="25">
         <v>25.8</v>
       </c>
-      <c r="I4" s="84">
-        <v>0.18408141013992368</v>
+      <c r="I4" s="72">
+        <v>0.25945727832139615</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3345,7 +3363,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="25">
-        <v>51</v>
+        <v>57.4</v>
       </c>
       <c r="C5" t="s">
         <v>136</v>
@@ -3362,8 +3380,8 @@
       <c r="H5" s="25">
         <v>55.5</v>
       </c>
-      <c r="I5" s="84">
-        <v>0.50999454842813008</v>
+      <c r="I5" s="72">
+        <v>0.57389286795117522</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3371,7 +3389,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="25">
-        <v>24.8</v>
+        <v>13.5</v>
       </c>
       <c r="C6" t="s">
         <v>137</v>
@@ -3388,8 +3406,8 @@
       <c r="H6" s="25">
         <v>15.2</v>
       </c>
-      <c r="I6" s="84">
-        <v>0.2476376521897147</v>
+      <c r="I6" s="72">
+        <v>0.13477252093210934</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3397,7 +3415,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="25">
-        <v>5</v>
+        <v>1.9</v>
       </c>
       <c r="C7" t="s">
         <v>138</v>
@@ -3405,8 +3423,8 @@
       <c r="H7" s="25">
         <v>2.1</v>
       </c>
-      <c r="I7" s="84">
-        <v>0.05</v>
+      <c r="I7" s="72">
+        <v>1.9267628366791082E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -5266,7 +5284,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5374,7 +5392,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="25">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J4" s="69">
         <v>46</v>
@@ -5398,7 +5416,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="25">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="J5" s="69">
         <v>53</v>
@@ -5826,7 +5844,7 @@
       </c>
       <c r="K4" s="25">
         <f>'Routes Zone (1) Major'!I4</f>
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -5856,7 +5874,7 @@
       </c>
       <c r="K5" s="25">
         <f>'Routes Zone (1) Major'!I5</f>
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -7482,10 +7500,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7499,7 +7517,7 @@
     <col min="9" max="9" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -7521,9 +7539,8 @@
       <c r="I1" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -7545,9 +7562,8 @@
       <c r="I2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -7567,13 +7583,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="25">
-        <v>33</v>
-      </c>
-      <c r="J3" s="69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -7593,13 +7606,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="25">
-        <v>49</v>
-      </c>
-      <c r="J4" s="69">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -7617,13 +7627,10 @@
         <v>2</v>
       </c>
       <c r="I5" s="25">
-        <v>18</v>
-      </c>
-      <c r="J5" s="69">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -7642,7 +7649,7 @@
       </c>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -7656,7 +7663,7 @@
       </c>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -7670,7 +7677,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -7684,7 +7691,7 @@
       </c>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -7698,7 +7705,7 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -7712,7 +7719,7 @@
       </c>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -7726,7 +7733,7 @@
       </c>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -7740,7 +7747,7 @@
       </c>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -7754,7 +7761,7 @@
       </c>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -7768,7 +7775,7 @@
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -7916,7 +7923,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7968,7 +7975,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="25">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>89</v>
@@ -7985,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="25">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F4" s="48" t="s">
         <v>104</v>
@@ -8015,7 +8022,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="25">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F6" s="48" t="s">
         <v>91</v>
@@ -8030,7 +8037,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="48" t="s">
         <v>110</v>
@@ -8045,7 +8052,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="25">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="F8" s="48" t="s">
         <v>92</v>
@@ -8224,9 +8231,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X18"/>
+  <dimension ref="B1:X19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8242,34 +8251,34 @@
   <sheetData>
     <row r="1" spans="2:24" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>9.5384412103388048</v>
+        <v>8.7119770951926316</v>
       </c>
       <c r="C1" s="68">
-        <v>13.152080289277446</v>
+        <v>13.706311120856585</v>
       </c>
       <c r="D1" s="68">
-        <v>6.6752552815003963</v>
+        <v>5.9029223909316206</v>
       </c>
       <c r="E1" s="68">
-        <v>32.27373280754064</v>
+        <v>35.795935647756139</v>
       </c>
       <c r="F1" s="68">
-        <v>51.089204135609521</v>
+        <v>58.344798391364158</v>
       </c>
       <c r="G1" s="68">
-        <v>55.925191760751524</v>
+        <v>55.720899470899468</v>
       </c>
       <c r="H1" s="68">
-        <v>74.982764563943476</v>
+        <v>84.046949909075892</v>
       </c>
       <c r="I1" s="68">
-        <v>0.89569882695280534</v>
+        <v>0.86594055374592838</v>
       </c>
       <c r="J1" s="68">
-        <v>0.44162044193871058</v>
+        <v>0.34710912052117265</v>
       </c>
       <c r="K1" s="68">
-        <v>6.4335727925797948E-2</v>
+        <v>9.6498371335504887E-2</v>
       </c>
       <c r="O1" s="68">
         <v>9.3255076414271194</v>
@@ -8637,43 +8646,43 @@
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B5)</f>
-        <v>17.173123176136759</v>
+        <v>17.007830353107519</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:K13" si="0">AVERAGE(C1:C5)</f>
-        <v>28.294032395178522</v>
+        <v>28.40487856149435</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>6.8796892057322028</v>
+        <v>6.7252226276184475</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>25.840959792103241</v>
+        <v>26.545400360146338</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>40.212060014368411</v>
+        <v>41.663178865519335</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>48.488219787146463</v>
+        <v>48.447361329176054</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>71.189312683288236</v>
+        <v>73.002149752314708</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.92242120693470009</v>
+        <v>0.91646955229332472</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.48196828259592295</v>
+        <v>0.46306601831241528</v>
       </c>
       <c r="K13" s="67">
         <f t="shared" si="0"/>
-        <v>3.7368872338793734E-2</v>
+        <v>4.3801401020735126E-2</v>
       </c>
       <c r="O13" s="67">
         <f>AVERAGE(O1:O5)</f>
@@ -8748,8 +8757,49 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:11" s="70" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f>B18*0.95</f>
+        <v>9.5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:K17" si="2">C18*0.95</f>
+        <v>15.2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>6.3650000000000002</v>
+      </c>
+      <c r="E17" s="85">
+        <f t="shared" si="2"/>
+        <v>0.30419949999999996</v>
+      </c>
+      <c r="F17" s="85">
+        <f t="shared" si="2"/>
+        <v>0.53417549999999991</v>
+      </c>
+      <c r="G17" s="85">
+        <f t="shared" si="2"/>
+        <v>0.44670900000000002</v>
+      </c>
+      <c r="H17" s="85">
+        <f t="shared" si="2"/>
+        <v>0.73765599999999987</v>
+      </c>
+      <c r="I17" s="85">
+        <f t="shared" si="2"/>
+        <v>0.85024999999999995</v>
+      </c>
+      <c r="J17" s="85">
+        <f t="shared" si="2"/>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="K17" s="85">
+        <f t="shared" si="2"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" s="70" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="70">
         <v>10</v>
       </c>
@@ -8780,6 +8830,49 @@
       <c r="K18" s="70">
         <v>0.1</v>
       </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f>B18*1.05</f>
+        <v>10.5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:K19" si="3">C18*1.05</f>
+        <v>16.8</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>7.0350000000000001</v>
+      </c>
+      <c r="E19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.33622050000000003</v>
+      </c>
+      <c r="F19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.5904045</v>
+      </c>
+      <c r="G19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.49373100000000003</v>
+      </c>
+      <c r="H19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.81530400000000003</v>
+      </c>
+      <c r="I19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.93975000000000009</v>
+      </c>
+      <c r="J19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="K19" s="85">
+        <f t="shared" si="3"/>
+        <v>0.10500000000000001</v>
+      </c>
+      <c r="L19" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9782,7 +9875,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="79" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -9817,7 +9910,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+      <c r="A20" s="80"/>
       <c r="B20" s="8">
         <v>2</v>
       </c>
@@ -9850,7 +9943,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -9898,9 +9991,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10287,12 +10378,18 @@
       <c r="B14" s="5">
         <v>13</v>
       </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15">
         <v>2</v>
       </c>
     </row>
@@ -10330,7 +10427,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="81" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -10340,7 +10437,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="9">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E19" s="61"/>
       <c r="F19" s="61">
@@ -10353,7 +10450,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="10">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="J19" s="10">
         <v>1</v>
@@ -10366,7 +10463,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="81"/>
+      <c r="A20" s="82"/>
       <c r="B20" s="8">
         <v>7</v>
       </c>
@@ -10374,7 +10471,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="9">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E20" s="61"/>
       <c r="F20" s="61">
@@ -10387,7 +10484,7 @@
         <v>15</v>
       </c>
       <c r="I20" s="10">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J20" s="10">
         <v>7</v>
@@ -10396,11 +10493,11 @@
         <v>106</v>
       </c>
       <c r="L20" s="55">
-        <v>300</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="82"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -10408,7 +10505,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="9">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E21" s="61"/>
       <c r="F21" s="61">
@@ -10421,7 +10518,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="10">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="J21" s="10">
         <v>5</v>
@@ -10914,7 +11011,7 @@
       </c>
       <c r="B15" s="5">
         <f>'ZONE (1) MAJOR'!B15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -10928,10 +11025,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11325,6 +11422,9 @@
         <v>22</v>
       </c>
       <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15">
         <v>3</v>
       </c>
     </row>
@@ -11362,7 +11462,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="81" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -11379,13 +11479,13 @@
         <v>30</v>
       </c>
       <c r="G19" s="10">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H19" s="10">
         <v>5</v>
       </c>
       <c r="I19" s="10">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="J19" s="10">
         <v>1</v>
@@ -11394,11 +11494,11 @@
         <v>105</v>
       </c>
       <c r="L19" s="55">
-        <v>150</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="81"/>
+      <c r="A20" s="82"/>
       <c r="B20" s="8">
         <v>7</v>
       </c>
@@ -11413,13 +11513,13 @@
         <v>30</v>
       </c>
       <c r="G20" s="10">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H20" s="10">
         <v>15</v>
       </c>
       <c r="I20" s="10">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="J20" s="10">
         <v>7</v>
@@ -11428,11 +11528,11 @@
         <v>106</v>
       </c>
       <c r="L20" s="55">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="82"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -11447,13 +11547,13 @@
         <v>30</v>
       </c>
       <c r="G21" s="10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H21" s="10">
         <v>10</v>
       </c>
       <c r="I21" s="10">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J21" s="10">
         <v>5</v>
@@ -11462,7 +11562,31 @@
         <v>107</v>
       </c>
       <c r="L21" s="55">
-        <v>180</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G23" s="10">
+        <v>5</v>
+      </c>
+      <c r="I23" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G24" s="10">
+        <v>15</v>
+      </c>
+      <c r="I24" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G25" s="10">
+        <v>10</v>
+      </c>
+      <c r="I25" s="10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates on 28-Nov for 3-Dec
The SSU capacity is 24, should be 12
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,62 +4,66 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
   </bookViews>
   <sheets>
-    <sheet name="Sim Runs" sheetId="29" r:id="rId1"/>
-    <sheet name="Output" sheetId="27" r:id="rId2"/>
-    <sheet name="Interface" sheetId="20" r:id="rId3"/>
-    <sheet name="Zone1" sheetId="1" state="hidden" r:id="rId4"/>
-    <sheet name="Resus" sheetId="21" r:id="rId5"/>
-    <sheet name="ZONE (1) MAJOR" sheetId="23" r:id="rId6"/>
-    <sheet name="Zone2" sheetId="2" state="hidden" r:id="rId7"/>
-    <sheet name="AMAU" sheetId="31" r:id="rId8"/>
-    <sheet name="Minor" sheetId="22" r:id="rId9"/>
-    <sheet name="Zone3" sheetId="3" state="hidden" r:id="rId10"/>
-    <sheet name="Discharge Waiting Time" sheetId="17" r:id="rId11"/>
-    <sheet name="Other Processes Timing" sheetId="18" r:id="rId12"/>
-    <sheet name="Resources" sheetId="4" r:id="rId13"/>
-    <sheet name="Resources_AMAU" sheetId="30" r:id="rId14"/>
-    <sheet name="Scans, Imaging and Tests" sheetId="28" r:id="rId15"/>
-    <sheet name="Routes Patient Arrival" sheetId="11" r:id="rId16"/>
-    <sheet name="Routes Triage" sheetId="10" r:id="rId17"/>
-    <sheet name="Routes RAT" sheetId="9" state="hidden" r:id="rId18"/>
-    <sheet name="Routes RESUS" sheetId="24" r:id="rId19"/>
-    <sheet name="Routes Zone1" sheetId="6" state="hidden" r:id="rId20"/>
-    <sheet name="Routes Zone (1) Major" sheetId="25" r:id="rId21"/>
-    <sheet name="Routes Zone2" sheetId="7" state="hidden" r:id="rId22"/>
-    <sheet name="Routes Minor" sheetId="26" r:id="rId23"/>
-    <sheet name="Routes Zone3" sheetId="8" state="hidden" r:id="rId24"/>
-    <sheet name="Routes AMAU" sheetId="32" r:id="rId25"/>
-    <sheet name="Routes Discharge" sheetId="16" r:id="rId26"/>
+    <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
+    <sheet name="Sim Runs" sheetId="29" r:id="rId2"/>
+    <sheet name="Output" sheetId="27" r:id="rId3"/>
+    <sheet name="Interface" sheetId="20" r:id="rId4"/>
+    <sheet name="Zone1" sheetId="1" state="hidden" r:id="rId5"/>
+    <sheet name="Resus" sheetId="21" r:id="rId6"/>
+    <sheet name="ZONE (1) MAJOR" sheetId="23" r:id="rId7"/>
+    <sheet name="Zone2" sheetId="2" state="hidden" r:id="rId8"/>
+    <sheet name="AMAU" sheetId="31" r:id="rId9"/>
+    <sheet name="Minor" sheetId="22" r:id="rId10"/>
+    <sheet name="Zone3" sheetId="3" state="hidden" r:id="rId11"/>
+    <sheet name="Discharge Waiting Time" sheetId="17" r:id="rId12"/>
+    <sheet name="Other Processes Timing" sheetId="18" r:id="rId13"/>
+    <sheet name="Resources" sheetId="4" r:id="rId14"/>
+    <sheet name="Resources_AMAU" sheetId="30" r:id="rId15"/>
+    <sheet name="Scans, Imaging and Tests" sheetId="28" r:id="rId16"/>
+    <sheet name="Routes Patient Arrival" sheetId="11" r:id="rId17"/>
+    <sheet name="Routes Triage" sheetId="10" r:id="rId18"/>
+    <sheet name="Routes RAT" sheetId="9" state="hidden" r:id="rId19"/>
+    <sheet name="Routes RESUS" sheetId="24" r:id="rId20"/>
+    <sheet name="Routes Zone1" sheetId="6" state="hidden" r:id="rId21"/>
+    <sheet name="Routes Zone (1) Major" sheetId="25" r:id="rId22"/>
+    <sheet name="Routes Zone2" sheetId="7" state="hidden" r:id="rId23"/>
+    <sheet name="Routes Minor" sheetId="26" r:id="rId24"/>
+    <sheet name="Routes Zone3" sheetId="8" state="hidden" r:id="rId25"/>
+    <sheet name="Routes AMAU" sheetId="32" r:id="rId26"/>
+    <sheet name="Routes Discharge" sheetId="16" r:id="rId27"/>
   </sheets>
   <definedNames>
-    <definedName name="Prob" localSheetId="7">#REF!</definedName>
     <definedName name="Prob" localSheetId="8">#REF!</definedName>
-    <definedName name="Prob" localSheetId="13">#REF!</definedName>
-    <definedName name="Prob" localSheetId="4">#REF!</definedName>
-    <definedName name="Prob" localSheetId="24">#REF!</definedName>
-    <definedName name="Prob" localSheetId="22">#REF!</definedName>
-    <definedName name="Prob" localSheetId="18">#REF!</definedName>
-    <definedName name="Prob" localSheetId="20">#REF!</definedName>
+    <definedName name="Prob" localSheetId="9">#REF!</definedName>
     <definedName name="Prob" localSheetId="14">#REF!</definedName>
     <definedName name="Prob" localSheetId="5">#REF!</definedName>
+    <definedName name="Prob" localSheetId="25">#REF!</definedName>
+    <definedName name="Prob" localSheetId="23">#REF!</definedName>
+    <definedName name="Prob" localSheetId="19">#REF!</definedName>
+    <definedName name="Prob" localSheetId="21">#REF!</definedName>
+    <definedName name="Prob" localSheetId="15">#REF!</definedName>
+    <definedName name="Prob" localSheetId="0">#REF!</definedName>
+    <definedName name="Prob" localSheetId="6">#REF!</definedName>
     <definedName name="Prob">#REF!</definedName>
-    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="7">#REF!</definedName>
-    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="13">#REF!</definedName>
-    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="24">#REF!</definedName>
+    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="8">#REF!</definedName>
+    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="14">#REF!</definedName>
+    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="25">#REF!</definedName>
+    <definedName name="Scans_Imaging_Tests_Routes" localSheetId="0">#REF!</definedName>
     <definedName name="Scans_Imaging_Tests_Routes">#REF!</definedName>
-    <definedName name="Values" localSheetId="7">#REF!</definedName>
     <definedName name="Values" localSheetId="8">#REF!</definedName>
-    <definedName name="Values" localSheetId="13">#REF!</definedName>
-    <definedName name="Values" localSheetId="4">#REF!</definedName>
-    <definedName name="Values" localSheetId="24">#REF!</definedName>
-    <definedName name="Values" localSheetId="22">#REF!</definedName>
-    <definedName name="Values" localSheetId="18">#REF!</definedName>
-    <definedName name="Values" localSheetId="20">#REF!</definedName>
+    <definedName name="Values" localSheetId="9">#REF!</definedName>
     <definedName name="Values" localSheetId="14">#REF!</definedName>
     <definedName name="Values" localSheetId="5">#REF!</definedName>
+    <definedName name="Values" localSheetId="25">#REF!</definedName>
+    <definedName name="Values" localSheetId="23">#REF!</definedName>
+    <definedName name="Values" localSheetId="19">#REF!</definedName>
+    <definedName name="Values" localSheetId="21">#REF!</definedName>
+    <definedName name="Values" localSheetId="15">#REF!</definedName>
+    <definedName name="Values" localSheetId="0">#REF!</definedName>
+    <definedName name="Values" localSheetId="6">#REF!</definedName>
     <definedName name="Values">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -67,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="142">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -1438,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1454,35 +1458,27 @@
   <sheetData>
     <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>10.736851060297745</v>
+        <v>7.8627395833627807</v>
       </c>
       <c r="C1" s="68">
-        <v>18.479938396185471</v>
+        <v>15.954872838108887</v>
       </c>
       <c r="D1" s="68">
-        <v>8.0950578100489547</v>
+        <v>5.5956782419622533</v>
       </c>
       <c r="E1" s="68">
-        <v>34.382690253981515</v>
+        <v>10.006920120288763</v>
       </c>
       <c r="F1" s="68">
-        <v>42.306620856161203</v>
+        <v>16.010414520015136</v>
       </c>
       <c r="G1" s="68">
-        <v>45.967993025717668</v>
-      </c>
-      <c r="H1" s="68">
-        <v>55.261519302615191</v>
-      </c>
-      <c r="I1" s="68">
-        <v>0.90027272727272722</v>
-      </c>
-      <c r="J1" s="68">
-        <v>0.25036363636363634</v>
-      </c>
-      <c r="K1" s="68">
-        <v>7.9909090909090916E-2</v>
-      </c>
+        <v>7.5926034483987106</v>
+      </c>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
@@ -1619,43 +1615,43 @@
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>10.736851060297745</v>
+        <v>7.8627395833627807</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>18.479938396185471</v>
+        <v>15.954872838108887</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>8.0950578100489547</v>
+        <v>5.5956782419622533</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>34.382690253981515</v>
+        <v>10.006920120288763</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>42.306620856161203</v>
+        <v>16.010414520015136</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>45.967993025717668</v>
-      </c>
-      <c r="H13" s="67">
+        <v>7.5926034483987106</v>
+      </c>
+      <c r="H13" s="67" t="e">
         <f t="shared" si="0"/>
-        <v>55.261519302615191</v>
-      </c>
-      <c r="I13" s="67">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="67" t="e">
         <f t="shared" si="0"/>
-        <v>0.90027272727272722</v>
-      </c>
-      <c r="J13" s="67">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="67" t="e">
         <f t="shared" si="0"/>
-        <v>0.25036363636363634</v>
-      </c>
-      <c r="K13" s="67">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="67" t="e">
         <f>AVERAGE(K1:K10)</f>
-        <v>7.9909090909090916E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1748,6 +1744,540 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="61">
+        <v>5</v>
+      </c>
+      <c r="C2" s="61">
+        <v>10</v>
+      </c>
+      <c r="D2" s="61">
+        <v>30</v>
+      </c>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61">
+        <v>30</v>
+      </c>
+      <c r="G2" s="61">
+        <v>5</v>
+      </c>
+      <c r="H2" s="61">
+        <v>10</v>
+      </c>
+      <c r="I2" s="61">
+        <v>10</v>
+      </c>
+      <c r="J2" s="61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11">
+        <v>1</v>
+      </c>
+      <c r="J6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="61">
+        <v>0</v>
+      </c>
+      <c r="C9" s="61">
+        <v>0</v>
+      </c>
+      <c r="D9" s="61">
+        <v>0</v>
+      </c>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61">
+        <v>0</v>
+      </c>
+      <c r="G9" s="61">
+        <v>0</v>
+      </c>
+      <c r="H9" s="61">
+        <v>0</v>
+      </c>
+      <c r="I9" s="61">
+        <v>0</v>
+      </c>
+      <c r="J9" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="61">
+        <v>0</v>
+      </c>
+      <c r="C12" s="61">
+        <v>0</v>
+      </c>
+      <c r="D12" s="61">
+        <v>0</v>
+      </c>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61">
+        <v>0</v>
+      </c>
+      <c r="G12" s="61">
+        <v>0</v>
+      </c>
+      <c r="H12" s="61">
+        <v>0</v>
+      </c>
+      <c r="I12" s="61">
+        <v>0</v>
+      </c>
+      <c r="J12" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="61"/>
+      <c r="F18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9">
+        <v>10</v>
+      </c>
+      <c r="E19" s="61"/>
+      <c r="F19" s="10">
+        <v>10</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1</v>
+      </c>
+      <c r="H19" s="10">
+        <v>5</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="8">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9">
+        <v>7</v>
+      </c>
+      <c r="D20" s="9">
+        <v>30</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="10">
+        <v>30</v>
+      </c>
+      <c r="G20" s="10">
+        <v>7</v>
+      </c>
+      <c r="H20" s="10">
+        <v>15</v>
+      </c>
+      <c r="I20" s="10">
+        <v>2</v>
+      </c>
+      <c r="J20" s="10">
+        <v>2</v>
+      </c>
+      <c r="K20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="53"/>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>5</v>
+      </c>
+      <c r="D21" s="9">
+        <v>20</v>
+      </c>
+      <c r="E21" s="61"/>
+      <c r="F21" s="10">
+        <v>20</v>
+      </c>
+      <c r="G21" s="10">
+        <v>5</v>
+      </c>
+      <c r="H21" s="10">
+        <v>10</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
@@ -2274,7 +2804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -2478,7 +3008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -2637,7 +3167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -2645,7 +3175,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,7 +3378,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="12">
         <v>7</v>
@@ -2871,7 +3401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -3105,7 +3635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -3490,14 +4020,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3912,7 +4442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -4179,7 +4709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
@@ -4593,7 +5123,320 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L19"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="68">
+        <v>9.0944320840848221</v>
+      </c>
+      <c r="C1" s="68">
+        <v>17.165287298497564</v>
+      </c>
+      <c r="D1" s="68">
+        <v>6.8333319177096756</v>
+      </c>
+      <c r="E1" s="68">
+        <v>45.719448836683988</v>
+      </c>
+      <c r="F1" s="68">
+        <v>54.737436476566913</v>
+      </c>
+      <c r="G1" s="68">
+        <v>58.377909498337431</v>
+      </c>
+      <c r="H1" s="68">
+        <v>68.459092223185891</v>
+      </c>
+      <c r="I1" s="68">
+        <v>0.93427315171569736</v>
+      </c>
+      <c r="J1" s="68">
+        <v>0.27682335342912834</v>
+      </c>
+      <c r="K1" s="68">
+        <v>4.5691491772811746E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="67">
+        <f>AVERAGE(B1:B10)</f>
+        <v>9.0944320840848221</v>
+      </c>
+      <c r="C13" s="67">
+        <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
+        <v>17.165287298497564</v>
+      </c>
+      <c r="D13" s="67">
+        <f t="shared" si="0"/>
+        <v>6.8333319177096756</v>
+      </c>
+      <c r="E13" s="67">
+        <f t="shared" si="0"/>
+        <v>45.719448836683988</v>
+      </c>
+      <c r="F13" s="67">
+        <f t="shared" si="0"/>
+        <v>54.737436476566913</v>
+      </c>
+      <c r="G13" s="67">
+        <f t="shared" si="0"/>
+        <v>58.377909498337431</v>
+      </c>
+      <c r="H13" s="67">
+        <f t="shared" si="0"/>
+        <v>68.459092223185891</v>
+      </c>
+      <c r="I13" s="67">
+        <f t="shared" si="0"/>
+        <v>0.93427315171569736</v>
+      </c>
+      <c r="J13" s="67">
+        <f t="shared" si="0"/>
+        <v>0.27682335342912834</v>
+      </c>
+      <c r="K13" s="67">
+        <f>AVERAGE(K1:K10)</f>
+        <v>4.5691491772811746E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="K16" s="63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+    </row>
+    <row r="18" spans="2:12" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="70">
+        <v>10</v>
+      </c>
+      <c r="C18" s="70">
+        <v>16</v>
+      </c>
+      <c r="D18" s="70">
+        <v>6.7</v>
+      </c>
+      <c r="E18" s="71">
+        <v>0.32020999999999999</v>
+      </c>
+      <c r="F18" s="71">
+        <v>0.56228999999999996</v>
+      </c>
+      <c r="G18" s="71">
+        <v>0.47022000000000003</v>
+      </c>
+      <c r="H18" s="71">
+        <v>0.77647999999999995</v>
+      </c>
+      <c r="I18" s="71">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J18" s="71">
+        <v>0.38</v>
+      </c>
+      <c r="K18" s="74">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -4992,278 +5835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="80"/>
-      <c r="G1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="38">
-        <v>0.16666284201910753</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="36">
-        <v>0.662909858172124</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="37">
-        <v>644.21106361786474</v>
-      </c>
-      <c r="G2">
-        <f>F2/1440</f>
-        <v>0.44736879417907272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="46">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="36">
-        <v>0.50982360376345159</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="37">
-        <v>34.39487488974514</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="38">
-        <v>0.17795801526717558</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="36">
-        <v>6.662547540024899E-2</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="37">
-        <v>42.317333580911708</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="38">
-        <v>0.96615950322979594</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="36">
-        <v>0.5889540139695264</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="37">
-        <v>7.1697321491013239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="38">
-        <v>0.35911193339500619</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="36">
-        <v>0.19379685091332111</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="37">
-        <v>350.27100910207253</v>
-      </c>
-      <c r="G6">
-        <f>F6/1440</f>
-        <v>0.24324375632088369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="38">
-        <v>0.5579719933360342</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="36">
-        <v>0.45235883503105578</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="37">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f>F7/1440</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="36">
-        <v>0.36157536114387739</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="37">
-        <v>0.22710895079573046</v>
-      </c>
-      <c r="G8">
-        <f>F8/1440</f>
-        <v>1.577145491637017E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="78"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="36">
-        <v>0.11947977482718439</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="36">
-        <v>0.19419201596912697</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="36">
-        <v>0.26694461060780744</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="36">
-        <v>5.7440879497759376E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="36">
-        <v>0.13550488440274772</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C12:D12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6172,7 +6744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -6603,7 +7175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
@@ -7348,7 +7920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -7645,7 +8217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
@@ -8391,7 +8963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -8811,7 +9383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -9130,6 +9702,277 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="80"/>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="38">
+        <v>0.16666285409279766</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="36">
+        <v>0.75657685244837247</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="37">
+        <v>545.66592504508935</v>
+      </c>
+      <c r="G2">
+        <f>F2/1440</f>
+        <v>0.37893467017020094</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="46">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.59439645738892399</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="37">
+        <v>45.743960261910139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="38">
+        <v>19.051446945337599</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="36">
+        <v>5.7333414581309576E-2</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="37">
+        <v>54.757873349136474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="38">
+        <v>94.976248062015642</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="36">
+        <v>65.003935190078963</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="37">
+        <v>7.1217343351485551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="38">
+        <v>31.508243606998722</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="36">
+        <v>0.19478398225052967</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="37">
+        <v>333.27667540112117</v>
+      </c>
+      <c r="G6">
+        <f>F6/1440</f>
+        <v>0.23144213569522304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="38">
+        <v>78.554154430817064</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="36">
+        <v>0.42045244936900256</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="37">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>F7/1440</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="36">
+        <v>0.3762958341798785</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="37">
+        <v>1.1392918282565998</v>
+      </c>
+      <c r="G8">
+        <f>F8/1440</f>
+        <v>7.9117488073374989E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="78"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="36">
+        <v>0.24976841083136256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="36">
+        <v>0.3797136019648466</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="36">
+        <v>56.903679462665664</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="36">
+        <v>0.11148529644263477</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="36">
+        <v>0.48301888789830305</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C12:D12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9142,7 +9985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J14"/>
@@ -9687,7 +10530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -10248,16 +11091,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10642,7 +11483,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -10716,7 +11557,7 @@
         <v>10</v>
       </c>
       <c r="I19" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="10">
         <v>1</v>
@@ -10750,7 +11591,7 @@
         <v>60</v>
       </c>
       <c r="I20" s="10">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J20" s="10">
         <v>7</v>
@@ -10784,7 +11625,7 @@
         <v>30</v>
       </c>
       <c r="I21" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J21" s="10">
         <v>5</v>
@@ -10805,7 +11646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J15"/>
@@ -11268,7 +12109,7 @@
       </c>
       <c r="B14" s="5">
         <f>'ZONE (1) MAJOR'!B14</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -11286,7 +12127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -11294,7 +12135,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11680,7 +12521,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="5">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -11751,7 +12592,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J19" s="10">
         <v>1</v>
@@ -11785,7 +12626,7 @@
         <v>20</v>
       </c>
       <c r="I20" s="10">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J20" s="10">
         <v>7</v>
@@ -11819,7 +12660,7 @@
         <v>15</v>
       </c>
       <c r="I21" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J21" s="10">
         <v>5</v>
@@ -11838,538 +12679,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.39997558519241921"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K21"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="61">
-        <v>5</v>
-      </c>
-      <c r="C2" s="61">
-        <v>10</v>
-      </c>
-      <c r="D2" s="61">
-        <v>30</v>
-      </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61">
-        <v>30</v>
-      </c>
-      <c r="G2" s="61">
-        <v>5</v>
-      </c>
-      <c r="H2" s="61">
-        <v>10</v>
-      </c>
-      <c r="I2" s="61">
-        <v>10</v>
-      </c>
-      <c r="J2" s="61">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="11">
-        <v>0</v>
-      </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0</v>
-      </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
-      <c r="J3" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
-      </c>
-      <c r="I4" s="11">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11">
-        <v>0</v>
-      </c>
-      <c r="C5" s="11">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1</v>
-      </c>
-      <c r="I5" s="11">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>0</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11">
-        <v>1</v>
-      </c>
-      <c r="J6" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61">
-        <v>1</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11">
-        <v>1</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11">
-        <v>0</v>
-      </c>
-      <c r="C8" s="11">
-        <v>0</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="61">
-        <v>0</v>
-      </c>
-      <c r="C9" s="61">
-        <v>0</v>
-      </c>
-      <c r="D9" s="61">
-        <v>0</v>
-      </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61">
-        <v>0</v>
-      </c>
-      <c r="G9" s="61">
-        <v>0</v>
-      </c>
-      <c r="H9" s="61">
-        <v>0</v>
-      </c>
-      <c r="I9" s="61">
-        <v>0</v>
-      </c>
-      <c r="J9" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="11">
-        <v>0</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61">
-        <v>1</v>
-      </c>
-      <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="11">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61">
-        <v>0</v>
-      </c>
-      <c r="G11" s="11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="61">
-        <v>0</v>
-      </c>
-      <c r="C12" s="61">
-        <v>0</v>
-      </c>
-      <c r="D12" s="61">
-        <v>0</v>
-      </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61">
-        <v>0</v>
-      </c>
-      <c r="G12" s="61">
-        <v>0</v>
-      </c>
-      <c r="H12" s="61">
-        <v>0</v>
-      </c>
-      <c r="I12" s="61">
-        <v>0</v>
-      </c>
-      <c r="J12" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="5">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9">
-        <v>10</v>
-      </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="10">
-        <v>10</v>
-      </c>
-      <c r="G19" s="10">
-        <v>1</v>
-      </c>
-      <c r="H19" s="10">
-        <v>5</v>
-      </c>
-      <c r="I19" s="10">
-        <v>1</v>
-      </c>
-      <c r="J19" s="10">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
-      <c r="B20" s="8">
-        <v>2</v>
-      </c>
-      <c r="C20" s="9">
-        <v>7</v>
-      </c>
-      <c r="D20" s="9">
-        <v>30</v>
-      </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="10">
-        <v>30</v>
-      </c>
-      <c r="G20" s="10">
-        <v>7</v>
-      </c>
-      <c r="H20" s="10">
-        <v>15</v>
-      </c>
-      <c r="I20" s="10">
-        <v>2</v>
-      </c>
-      <c r="J20" s="10">
-        <v>2</v>
-      </c>
-      <c r="K20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
-      <c r="B21" s="8">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9">
-        <v>5</v>
-      </c>
-      <c r="D21" s="9">
-        <v>20</v>
-      </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="10">
-        <v>20</v>
-      </c>
-      <c r="G21" s="10">
-        <v>5</v>
-      </c>
-      <c r="H21" s="10">
-        <v>10</v>
-      </c>
-      <c r="I21" s="10">
-        <v>1</v>
-      </c>
-      <c r="J21" s="10">
-        <v>1</v>
-      </c>
-      <c r="K21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Include the time of the AMAU patients
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="151">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -497,6 +497,33 @@
   </si>
   <si>
     <t>From Data of ED + AMAU</t>
+  </si>
+  <si>
+    <t>PET (All-Non)</t>
+  </si>
+  <si>
+    <t>PET (Adm-Non)</t>
+  </si>
+  <si>
+    <t>PET (Disch.-Non)</t>
+  </si>
+  <si>
+    <t>PET (All-MED)</t>
+  </si>
+  <si>
+    <t>PET (Adm-Med)</t>
+  </si>
+  <si>
+    <t>PET (Disch.-Med)</t>
+  </si>
+  <si>
+    <t>PET (All-AMAU)</t>
+  </si>
+  <si>
+    <t>PET (Adm-AMAU)</t>
+  </si>
+  <si>
+    <t>PET (Disch.-AMAU)</t>
   </si>
 </sst>
 </file>
@@ -1440,23 +1467,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L19"/>
+  <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:S1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
         <v>7.8627395833627807</v>
       </c>
@@ -1478,9 +1508,26 @@
       <c r="H1" s="68"/>
       <c r="I1" s="68"/>
       <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N1" s="68">
+        <v>7.8627395833627807</v>
+      </c>
+      <c r="O1" s="68">
+        <v>15.954872838108887</v>
+      </c>
+      <c r="P1" s="68">
+        <v>5.5956782419622533</v>
+      </c>
+      <c r="Q1" s="68">
+        <v>10.006920120288763</v>
+      </c>
+      <c r="R1" s="68">
+        <v>16.010414520015136</v>
+      </c>
+      <c r="S1" s="68">
+        <v>7.5926034483987106</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -1490,9 +1537,8 @@
       <c r="H2" s="68"/>
       <c r="I2" s="68"/>
       <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
       <c r="D3" s="68"/>
@@ -1502,9 +1548,8 @@
       <c r="H3" s="68"/>
       <c r="I3" s="68"/>
       <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="68"/>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
@@ -1514,9 +1559,8 @@
       <c r="H4" s="68"/>
       <c r="I4" s="68"/>
       <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
       <c r="D5" s="68"/>
@@ -1526,9 +1570,8 @@
       <c r="H5" s="68"/>
       <c r="I5" s="68"/>
       <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
       <c r="D6" s="68"/>
@@ -1538,9 +1581,8 @@
       <c r="H6" s="68"/>
       <c r="I6" s="68"/>
       <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="68"/>
       <c r="C7" s="68"/>
       <c r="D7" s="68"/>
@@ -1550,9 +1592,8 @@
       <c r="H7" s="68"/>
       <c r="I7" s="68"/>
       <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -1562,9 +1603,8 @@
       <c r="H8" s="68"/>
       <c r="I8" s="68"/>
       <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
@@ -1574,9 +1614,8 @@
       <c r="H9" s="68"/>
       <c r="I9" s="68"/>
       <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="68"/>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
@@ -1586,9 +1625,8 @@
       <c r="H10" s="68"/>
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="66"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
@@ -1598,9 +1636,8 @@
       <c r="H11" s="66"/>
       <c r="I11" s="66"/>
       <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
@@ -1610,9 +1647,8 @@
       <c r="H12" s="66"/>
       <c r="I12" s="66"/>
       <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
         <v>7.8627395833627807</v>
@@ -1649,85 +1685,53 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="67" t="e">
-        <f>AVERAGE(K1:K10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="63" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="F16" s="63" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="G16" s="63" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="I16" s="63" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="J16" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="K16" s="63" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E17" s="73"/>
       <c r="F17" s="73"/>
       <c r="G17" s="73"/>
       <c r="H17" s="73"/>
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-    </row>
-    <row r="18" spans="2:12" s="70" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="70">
-        <v>10</v>
-      </c>
-      <c r="C18" s="70">
-        <v>16</v>
-      </c>
-      <c r="D18" s="70">
-        <v>6.7</v>
-      </c>
-      <c r="E18" s="71">
-        <v>0.32020999999999999</v>
-      </c>
-      <c r="F18" s="71">
-        <v>0.56228999999999996</v>
-      </c>
-      <c r="G18" s="71">
-        <v>0.47022000000000003</v>
-      </c>
-      <c r="H18" s="71">
-        <v>0.77647999999999995</v>
-      </c>
-      <c r="I18" s="71">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="J18" s="71">
-        <v>0.38</v>
-      </c>
-      <c r="K18" s="74">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="5:11" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E19" s="73"/>
       <c r="F19" s="73"/>
       <c r="G19" s="73"/>
@@ -1735,7 +1739,6 @@
       <c r="I19" s="73"/>
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5125,9 +5128,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L19"/>
+  <dimension ref="B1:W19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:W2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5141,7 +5146,7 @@
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:23" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
         <v>9.0944320840848221</v>
       </c>
@@ -5172,8 +5177,38 @@
       <c r="K1" s="68">
         <v>4.5691491772811746E-2</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N1" s="68">
+        <v>9.0944320840848221</v>
+      </c>
+      <c r="O1" s="68">
+        <v>17.165287298497564</v>
+      </c>
+      <c r="P1" s="68">
+        <v>6.8333319177096756</v>
+      </c>
+      <c r="Q1" s="68">
+        <v>45.719448836683988</v>
+      </c>
+      <c r="R1" s="68">
+        <v>54.737436476566913</v>
+      </c>
+      <c r="S1" s="68">
+        <v>58.377909498337431</v>
+      </c>
+      <c r="T1" s="68">
+        <v>68.459092223185891</v>
+      </c>
+      <c r="U1" s="68">
+        <v>0.93427315171569736</v>
+      </c>
+      <c r="V1" s="68">
+        <v>0.27682335342912834</v>
+      </c>
+      <c r="W1" s="68">
+        <v>4.5691491772811746E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -5184,8 +5219,18 @@
       <c r="I2" s="68"/>
       <c r="J2" s="68"/>
       <c r="K2" s="68"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68"/>
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
       <c r="D3" s="68"/>
@@ -5197,7 +5242,7 @@
       <c r="J3" s="68"/>
       <c r="K3" s="68"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="68"/>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
@@ -5209,7 +5254,7 @@
       <c r="J4" s="68"/>
       <c r="K4" s="68"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
       <c r="D5" s="68"/>
@@ -5221,7 +5266,7 @@
       <c r="J5" s="68"/>
       <c r="K5" s="68"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
       <c r="D6" s="68"/>
@@ -5233,7 +5278,7 @@
       <c r="J6" s="68"/>
       <c r="K6" s="68"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="68"/>
       <c r="C7" s="68"/>
       <c r="D7" s="68"/>
@@ -5245,7 +5290,7 @@
       <c r="J7" s="68"/>
       <c r="K7" s="68"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -5257,7 +5302,7 @@
       <c r="J8" s="68"/>
       <c r="K8" s="68"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
@@ -5269,7 +5314,7 @@
       <c r="J9" s="68"/>
       <c r="K9" s="68"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B10" s="68"/>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
@@ -5281,7 +5326,7 @@
       <c r="J10" s="68"/>
       <c r="K10" s="68"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="66"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
@@ -5293,7 +5338,7 @@
       <c r="J11" s="66"/>
       <c r="K11" s="66"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
@@ -5305,7 +5350,7 @@
       <c r="J12" s="66"/>
       <c r="K12" s="66"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
         <v>9.0944320840848221</v>
@@ -5347,7 +5392,7 @@
         <v>4.5691491772811746E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="63" t="s">
         <v>124</v>
       </c>
@@ -9702,10 +9747,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9719,7 +9764,7 @@
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="s">
         <v>69</v>
       </c>
@@ -9735,8 +9780,23 @@
       <c r="G1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K1" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="76"/>
+      <c r="M1" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="78"/>
+      <c r="O1" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="80"/>
+      <c r="Q1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>64</v>
       </c>
@@ -9759,8 +9819,30 @@
         <f>F2/1440</f>
         <v>0.37893467017020094</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="38">
+        <v>0.16666285409279766</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="36">
+        <v>0.75657685244837247</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" s="37">
+        <v>545.66592504508935</v>
+      </c>
+      <c r="Q2">
+        <f>P2/1440</f>
+        <v>0.37893467017020094</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>56</v>
       </c>
@@ -9779,8 +9861,26 @@
       <c r="F3" s="37">
         <v>45.743960261910139</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K3" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="46">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="36">
+        <v>0.59439645738892399</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="37">
+        <v>45.743960261910139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>83</v>
       </c>
@@ -9799,8 +9899,26 @@
       <c r="F4" s="37">
         <v>54.757873349136474</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="38">
+        <v>19.051446945337599</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="36">
+        <v>5.7333414581309576E-2</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="37">
+        <v>54.757873349136474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>84</v>
       </c>
@@ -9819,8 +9937,26 @@
       <c r="F5" s="37">
         <v>7.1217343351485551</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K5" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="38">
+        <v>94.976248062015642</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="36">
+        <v>65.003935190078963</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="37">
+        <v>7.1217343351485551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
@@ -9843,8 +9979,30 @@
         <f>F6/1440</f>
         <v>0.23144213569522304</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K6" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="38">
+        <v>31.508243606998722</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="36">
+        <v>0.19478398225052967</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="P6" s="37">
+        <v>333.27667540112117</v>
+      </c>
+      <c r="Q6">
+        <f>P6/1440</f>
+        <v>0.23144213569522304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>103</v>
       </c>
@@ -9867,8 +10025,30 @@
         <f>F7/1440</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K7" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="38">
+        <v>78.554154430817064</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="36">
+        <v>0.42045244936900256</v>
+      </c>
+      <c r="O7" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>P7/1440</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C8" s="21" t="s">
         <v>7</v>
       </c>
@@ -9885,83 +10065,155 @@
         <f>F8/1440</f>
         <v>7.9117488073374989E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="36">
+        <v>0.3762958341798785</v>
+      </c>
+      <c r="O8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="37">
+        <v>1.1392918282565998</v>
+      </c>
+      <c r="Q8">
+        <f>P8/1440</f>
+        <v>7.9117488073374989E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9" s="43" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="47">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M9" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C12" s="77" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="78"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M12" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" s="78"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="36">
         <v>0.24976841083136256</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="36">
+        <v>0.24976841083136256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C14" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="36">
         <v>0.3797136019648466</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="36">
+        <v>0.3797136019648466</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C15" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="47">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M15" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C16" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D16" s="36">
         <v>56.903679462665664</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="M16" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="N16" s="36">
+        <v>56.903679462665664</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17" s="43" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="47">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="M17" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="N17" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C18" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="36">
         <v>0.11148529644263477</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="M18" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="36">
+        <v>0.11148529644263477</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="36">
         <v>0.48301888789830305</v>
       </c>
+      <c r="M19" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="36">
+        <v>0.48301888789830305</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="M12:N12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes in 29-Nov, reverted to old timings used in previous sheet
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="10656" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="153">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -524,6 +524,12 @@
   </si>
   <si>
     <t>PET (Disch.-AMAU)</t>
+  </si>
+  <si>
+    <t>Waiting Time for ED</t>
+  </si>
+  <si>
+    <t>Waiting Time for AMAU</t>
   </si>
 </sst>
 </file>
@@ -965,7 +971,7 @@
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1123,6 +1129,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1467,11 +1475,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S19"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:S1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1486,48 +1492,36 @@
     <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>7.8627395833627807</v>
+        <v>6.0960414944960748</v>
       </c>
       <c r="C1" s="68">
-        <v>15.954872838108887</v>
+        <v>15.927057241936573</v>
       </c>
       <c r="D1" s="68">
-        <v>5.5956782419622533</v>
+        <v>2.9005222305498846</v>
       </c>
       <c r="E1" s="68">
-        <v>10.006920120288763</v>
+        <v>7.6020925796009697</v>
       </c>
       <c r="F1" s="68">
-        <v>16.010414520015136</v>
+        <v>16.534918625538303</v>
       </c>
       <c r="G1" s="68">
-        <v>7.5926034483987106</v>
-      </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="N1" s="68">
-        <v>7.8627395833627807</v>
-      </c>
-      <c r="O1" s="68">
-        <v>15.954872838108887</v>
-      </c>
-      <c r="P1" s="68">
-        <v>5.5956782419622533</v>
-      </c>
-      <c r="Q1" s="68">
-        <v>10.006920120288763</v>
-      </c>
-      <c r="R1" s="68">
-        <v>16.010414520015136</v>
-      </c>
-      <c r="S1" s="68">
-        <v>7.5926034483987106</v>
-      </c>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+        <v>3.500132909047752</v>
+      </c>
+      <c r="H1" s="68">
+        <v>11.522614490050126</v>
+      </c>
+      <c r="I1" s="68">
+        <v>16.442613213024408</v>
+      </c>
+      <c r="J1" s="68">
+        <v>6.4460525618897409</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -1538,7 +1532,7 @@
       <c r="I2" s="68"/>
       <c r="J2" s="68"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
       <c r="D3" s="68"/>
@@ -1549,7 +1543,7 @@
       <c r="I3" s="68"/>
       <c r="J3" s="68"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="68"/>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
@@ -1560,7 +1554,7 @@
       <c r="I4" s="68"/>
       <c r="J4" s="68"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
       <c r="D5" s="68"/>
@@ -1571,7 +1565,7 @@
       <c r="I5" s="68"/>
       <c r="J5" s="68"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
       <c r="D6" s="68"/>
@@ -1582,7 +1576,7 @@
       <c r="I6" s="68"/>
       <c r="J6" s="68"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="68"/>
       <c r="C7" s="68"/>
       <c r="D7" s="68"/>
@@ -1593,7 +1587,7 @@
       <c r="I7" s="68"/>
       <c r="J7" s="68"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -1604,7 +1598,7 @@
       <c r="I8" s="68"/>
       <c r="J8" s="68"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
@@ -1615,7 +1609,7 @@
       <c r="I9" s="68"/>
       <c r="J9" s="68"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="68"/>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
@@ -1626,7 +1620,7 @@
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="66"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
@@ -1637,7 +1631,7 @@
       <c r="I11" s="66"/>
       <c r="J11" s="66"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
@@ -1648,45 +1642,45 @@
       <c r="I12" s="66"/>
       <c r="J12" s="66"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>7.8627395833627807</v>
+        <v>6.0960414944960748</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>15.954872838108887</v>
+        <v>15.927057241936573</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>5.5956782419622533</v>
+        <v>2.9005222305498846</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>10.006920120288763</v>
+        <v>7.6020925796009697</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>16.010414520015136</v>
+        <v>16.534918625538303</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>7.5926034483987106</v>
-      </c>
-      <c r="H13" s="67" t="e">
+        <v>3.500132909047752</v>
+      </c>
+      <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="67" t="e">
+        <v>11.522614490050126</v>
+      </c>
+      <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="67" t="e">
+        <v>16.442613213024408</v>
+      </c>
+      <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+        <v>6.4460525618897409</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="63" t="s">
         <v>142</v>
       </c>
@@ -1715,23 +1709,67 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="5:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-    </row>
-    <row r="18" spans="5:11" s="70" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="76">
+        <f t="shared" ref="B17:G17" si="1">B1-B18</f>
+        <v>6.0960414944960748</v>
+      </c>
+      <c r="C17" s="76">
+        <f t="shared" si="1"/>
+        <v>15.927057241936573</v>
+      </c>
+      <c r="D17" s="76">
+        <f t="shared" si="1"/>
+        <v>2.9005222305498846</v>
+      </c>
+      <c r="E17" s="76">
+        <f t="shared" si="1"/>
+        <v>-2.8079074203990304</v>
+      </c>
+      <c r="F17" s="76">
+        <f t="shared" si="1"/>
+        <v>0.17491862553830373</v>
+      </c>
+      <c r="G17" s="76">
+        <f t="shared" si="1"/>
+        <v>-3.2198670909522478</v>
+      </c>
+      <c r="H17" s="76">
+        <f>H1-H18</f>
+        <v>7.0626144900501258</v>
+      </c>
+      <c r="I17" s="76">
+        <f t="shared" ref="I17:J17" si="2">I1-I18</f>
+        <v>11.622613213024408</v>
+      </c>
+      <c r="J17" s="76">
+        <f t="shared" si="2"/>
+        <v>2.356052561889741</v>
+      </c>
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+    </row>
+    <row r="18" spans="2:12" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="75">
+        <v>10.41</v>
+      </c>
+      <c r="F18" s="75">
+        <v>16.36</v>
+      </c>
+      <c r="G18" s="75">
+        <v>6.72</v>
+      </c>
+      <c r="H18" s="75">
+        <v>4.46</v>
+      </c>
+      <c r="I18" s="75">
+        <v>4.82</v>
+      </c>
+      <c r="J18" s="75">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E19" s="73"/>
       <c r="F19" s="73"/>
       <c r="G19" s="73"/>
@@ -1755,7 +1793,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B19" sqref="B19:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,17 +2253,17 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="52"/>
       <c r="B20" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C20" s="9">
         <v>7</v>
       </c>
       <c r="D20" s="9">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E20" s="61"/>
       <c r="F20" s="10">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G20" s="10">
         <v>7</v>
@@ -2234,10 +2272,10 @@
         <v>15</v>
       </c>
       <c r="I20" s="10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J20" s="10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K20" t="s">
         <v>106</v>
@@ -2246,17 +2284,17 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
       <c r="B21" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21" s="9">
         <v>5</v>
       </c>
       <c r="D21" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E21" s="61"/>
       <c r="F21" s="10">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G21" s="10">
         <v>5</v>
@@ -2265,10 +2303,10 @@
         <v>10</v>
       </c>
       <c r="I21" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J21" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K21" t="s">
         <v>107</v>
@@ -2812,10 +2850,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2824,17 +2862,22 @@
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="76"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="77" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="88"/>
+      <c r="D1" s="78"/>
+      <c r="J1" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" s="88"/>
+      <c r="L1" s="78"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>50</v>
       </c>
@@ -2847,8 +2890,17 @@
       <c r="D2" s="65">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J2" s="65">
+        <v>150</v>
+      </c>
+      <c r="K2" s="65">
+        <v>120</v>
+      </c>
+      <c r="L2" s="65">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
@@ -2861,8 +2913,17 @@
       <c r="D3" s="45">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J3" s="45">
+        <v>90</v>
+      </c>
+      <c r="K3" s="45">
+        <v>90</v>
+      </c>
+      <c r="L3" s="45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>52</v>
       </c>
@@ -2875,14 +2936,26 @@
       <c r="D4" s="45">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J4" s="45">
+        <v>150</v>
+      </c>
+      <c r="K4" s="45">
+        <v>150</v>
+      </c>
+      <c r="L4" s="45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="62"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>58</v>
       </c>
@@ -2904,25 +2977,40 @@
       <c r="H6" s="30">
         <v>410</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J6" s="30">
+        <v>15</v>
+      </c>
+      <c r="K6" s="30">
+        <v>10</v>
+      </c>
+      <c r="L6" s="30">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="30">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="C9" s="30">
         <v>120</v>
@@ -2939,36 +3027,63 @@
       <c r="H9" s="30">
         <v>1400</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J9" s="30">
+        <v>90</v>
+      </c>
+      <c r="K9" s="30">
+        <v>30</v>
+      </c>
+      <c r="L9" s="30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="30">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C10" s="30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="30">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="J10" s="30">
+        <v>9</v>
+      </c>
+      <c r="K10" s="30">
+        <v>9</v>
+      </c>
+      <c r="L10" s="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="30">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C11" s="30">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D11" s="30">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="J11" s="30">
+        <v>4</v>
+      </c>
+      <c r="K11" s="30">
+        <v>4</v>
+      </c>
+      <c r="L11" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>62</v>
       </c>
@@ -2990,8 +3105,17 @@
       <c r="H12" s="30">
         <v>410</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J12" s="30">
+        <v>15</v>
+      </c>
+      <c r="K12" s="30">
+        <v>10</v>
+      </c>
+      <c r="L12" s="30">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>108</v>
       </c>
@@ -3003,8 +3127,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3019,7 +3144,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3032,11 +3157,11 @@
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="76"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="78"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -3049,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="30">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3071,13 +3196,13 @@
         <v>65</v>
       </c>
       <c r="B4" s="30">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C4" s="30">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" s="30">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3091,7 +3216,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="30">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3099,13 +3224,13 @@
         <v>112</v>
       </c>
       <c r="B6" s="30">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C6" s="30">
         <v>10</v>
       </c>
       <c r="D6" s="30">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3113,13 +3238,13 @@
         <v>113</v>
       </c>
       <c r="B7" s="30">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C7" s="30">
         <v>10</v>
       </c>
       <c r="D7" s="30">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3127,13 +3252,13 @@
         <v>114</v>
       </c>
       <c r="B8" s="30">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C8" s="30">
         <v>10</v>
       </c>
       <c r="D8" s="30">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3141,13 +3266,13 @@
         <v>115</v>
       </c>
       <c r="B9" s="30">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C9" s="30">
         <v>10</v>
       </c>
       <c r="D9" s="30">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3381,7 +3506,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="12">
         <v>7</v>
@@ -3412,7 +3537,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3615,7 +3740,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="12">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D18" s="12">
         <v>7</v>
@@ -4452,7 +4577,9 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5128,11 +5255,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W19"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:W2"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5146,69 +5271,39 @@
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>9.0944320840848221</v>
+        <v>7.2588821828366097</v>
       </c>
       <c r="C1" s="68">
-        <v>17.165287298497564</v>
+        <v>17.12105309406887</v>
       </c>
       <c r="D1" s="68">
-        <v>6.8333319177096756</v>
+        <v>4.0532360989741942</v>
       </c>
       <c r="E1" s="68">
-        <v>45.719448836683988</v>
+        <v>63.626151426645691</v>
       </c>
       <c r="F1" s="68">
-        <v>54.737436476566913</v>
+        <v>73.772885544198587</v>
       </c>
       <c r="G1" s="68">
-        <v>58.377909498337431</v>
+        <v>83.271320136925141</v>
       </c>
       <c r="H1" s="68">
-        <v>68.459092223185891</v>
+        <v>93.467261904761898</v>
       </c>
       <c r="I1" s="68">
-        <v>0.93427315171569736</v>
+        <v>0.97761329579511402</v>
       </c>
       <c r="J1" s="68">
-        <v>0.27682335342912834</v>
+        <v>0.29157206429933702</v>
       </c>
       <c r="K1" s="68">
-        <v>4.5691491772811746E-2</v>
-      </c>
-      <c r="N1" s="68">
-        <v>9.0944320840848221</v>
-      </c>
-      <c r="O1" s="68">
-        <v>17.165287298497564</v>
-      </c>
-      <c r="P1" s="68">
-        <v>6.8333319177096756</v>
-      </c>
-      <c r="Q1" s="68">
-        <v>45.719448836683988</v>
-      </c>
-      <c r="R1" s="68">
-        <v>54.737436476566913</v>
-      </c>
-      <c r="S1" s="68">
-        <v>58.377909498337431</v>
-      </c>
-      <c r="T1" s="68">
-        <v>68.459092223185891</v>
-      </c>
-      <c r="U1" s="68">
-        <v>0.93427315171569736</v>
-      </c>
-      <c r="V1" s="68">
-        <v>0.27682335342912834</v>
-      </c>
-      <c r="W1" s="68">
-        <v>4.5691491772811746E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+        <v>3.2240486785941333E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -5219,18 +5314,8 @@
       <c r="I2" s="68"/>
       <c r="J2" s="68"/>
       <c r="K2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
       <c r="D3" s="68"/>
@@ -5242,7 +5327,7 @@
       <c r="J3" s="68"/>
       <c r="K3" s="68"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="68"/>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
@@ -5254,7 +5339,7 @@
       <c r="J4" s="68"/>
       <c r="K4" s="68"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
       <c r="D5" s="68"/>
@@ -5266,7 +5351,7 @@
       <c r="J5" s="68"/>
       <c r="K5" s="68"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
       <c r="D6" s="68"/>
@@ -5278,7 +5363,7 @@
       <c r="J6" s="68"/>
       <c r="K6" s="68"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="68"/>
       <c r="C7" s="68"/>
       <c r="D7" s="68"/>
@@ -5290,7 +5375,7 @@
       <c r="J7" s="68"/>
       <c r="K7" s="68"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
       <c r="D8" s="68"/>
@@ -5302,7 +5387,7 @@
       <c r="J8" s="68"/>
       <c r="K8" s="68"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
       <c r="D9" s="68"/>
@@ -5314,7 +5399,7 @@
       <c r="J9" s="68"/>
       <c r="K9" s="68"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="68"/>
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
@@ -5326,7 +5411,7 @@
       <c r="J10" s="68"/>
       <c r="K10" s="68"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="66"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
@@ -5338,7 +5423,7 @@
       <c r="J11" s="66"/>
       <c r="K11" s="66"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
       <c r="D12" s="66"/>
@@ -5350,49 +5435,49 @@
       <c r="J12" s="66"/>
       <c r="K12" s="66"/>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>9.0944320840848221</v>
+        <v>7.2588821828366097</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>17.165287298497564</v>
+        <v>17.12105309406887</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>6.8333319177096756</v>
+        <v>4.0532360989741942</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>45.719448836683988</v>
+        <v>63.626151426645691</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>54.737436476566913</v>
+        <v>73.772885544198587</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>58.377909498337431</v>
+        <v>83.271320136925141</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>68.459092223185891</v>
+        <v>93.467261904761898</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.93427315171569736</v>
+        <v>0.97761329579511402</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.27682335342912834</v>
+        <v>0.29157206429933702</v>
       </c>
       <c r="K13" s="67">
         <f>AVERAGE(K1:K10)</f>
-        <v>4.5691491772811746E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
+        <v>3.2240486785941333E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="63" t="s">
         <v>124</v>
       </c>
@@ -9016,7 +9101,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9747,10 +9832,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9764,85 +9849,48 @@
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="77" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79" t="s">
+      <c r="D1" s="80"/>
+      <c r="E1" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="80"/>
+      <c r="F1" s="82"/>
       <c r="G1" t="s">
         <v>122</v>
       </c>
-      <c r="K1" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="76"/>
-      <c r="M1" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="80"/>
-      <c r="Q1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16666285409279766</v>
+        <v>0.1666628441243698</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>0.75657685244837247</v>
+        <v>0.3140476443322226</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>545.66592504508935</v>
+        <v>435.53293097019656</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>0.37893467017020094</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="38">
-        <v>0.16666285409279766</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="36">
-        <v>0.75657685244837247</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="P2" s="37">
-        <v>545.66592504508935</v>
-      </c>
-      <c r="Q2">
-        <f>P2/1440</f>
-        <v>0.37893467017020094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.30245342428485872</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>56</v>
       </c>
@@ -9853,167 +9901,91 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.59439645738892399</v>
+        <v>0.26660737728983663</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>45.743960261910139</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="46">
-        <v>0</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="36">
-        <v>0.59439645738892399</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" s="37">
-        <v>45.743960261910139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>63.642488210195367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>19.051446945337599</v>
+        <v>19.693396226415111</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>5.7333414581309576E-2</v>
+        <v>6.9624402390749587E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>54.757873349136474</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" s="38">
-        <v>19.051446945337599</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="36">
-        <v>5.7333414581309576E-2</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4" s="37">
-        <v>54.757873349136474</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>73.784663747614232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>94.976248062015642</v>
+        <v>80.578456258267508</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>65.003935190078963</v>
+        <v>36.714745333825597</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.1217343351485551</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="L5" s="38">
-        <v>94.976248062015642</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="N5" s="36">
-        <v>65.003935190078963</v>
-      </c>
-      <c r="O5" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="P5" s="37">
-        <v>7.1217343351485551</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>7.0919981467999635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>31.508243606998722</v>
+        <v>30.62366692261757</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.19478398225052967</v>
+        <v>0.18010653185241357</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>333.27667540112117</v>
+        <v>246.26884747269486</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>0.23144213569522304</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="L6" s="38">
-        <v>31.508243606998722</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" s="36">
-        <v>0.19478398225052967</v>
-      </c>
-      <c r="O6" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="P6" s="37">
-        <v>333.27667540112117</v>
-      </c>
-      <c r="Q6">
-        <f>P6/1440</f>
-        <v>0.23144213569522304</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.17102003296714921</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>103</v>
       </c>
       <c r="B7" s="38">
-        <v>78.554154430817064</v>
+        <v>57.405082712639619</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.42045244936900256</v>
+        <v>0.3146195250898039</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -10025,195 +9997,101 @@
         <f>F7/1440</f>
         <v>0</v>
       </c>
-      <c r="K7" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="L7" s="38">
-        <v>78.554154430817064</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="36">
-        <v>0.42045244936900256</v>
-      </c>
-      <c r="O7" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="P7" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <f>P7/1440</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>0.3762958341798785</v>
+        <v>0.38358215118247413</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>1.1392918282565998</v>
+        <v>0.12590771793231564</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>7.9117488073374989E-4</v>
-      </c>
-      <c r="M8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="36">
-        <v>0.3762958341798785</v>
-      </c>
-      <c r="O8" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="P8" s="37">
-        <v>1.1392918282565998</v>
-      </c>
-      <c r="Q8">
-        <f>P8/1440</f>
-        <v>7.9117488073374989E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>8.7435915230774759E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="43" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="47">
         <v>0</v>
       </c>
-      <c r="M9" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C12" s="77" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="M12" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="N12" s="78"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D12" s="80"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="36">
-        <v>0.24976841083136256</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N13" s="36">
-        <v>0.24976841083136256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.10503202477604377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="36">
-        <v>0.3797136019648466</v>
-      </c>
-      <c r="M14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="N14" s="36">
-        <v>0.3797136019648466</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.28910060035701884</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="47">
         <v>0</v>
       </c>
-      <c r="M15" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="N15" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D16" s="36">
-        <v>56.903679462665664</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="N16" s="36">
-        <v>56.903679462665664</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+        <v>41.040816357749726</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="43" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="47">
         <v>0</v>
       </c>
-      <c r="M17" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="N17" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="36">
-        <v>0.11148529644263477</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="N18" s="36">
-        <v>0.11148529644263477</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+        <v>5.3972767431266666E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="36">
-        <v>0.48301888789830305</v>
-      </c>
-      <c r="M19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="N19" s="36">
-        <v>0.48301888789830305</v>
+        <v>0.33102425018587123</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="M12:N12"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10790,7 +10668,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B19" sqref="B19:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11234,7 +11112,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="83" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
@@ -11256,7 +11134,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I19" s="10">
         <v>2</v>
@@ -11269,7 +11147,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="82"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="8">
         <v>2</v>
       </c>
@@ -11286,10 +11164,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="8">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="H20" s="8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I20" s="8">
         <v>7</v>
@@ -11302,7 +11180,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="82"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -11319,10 +11197,10 @@
         <v>15</v>
       </c>
       <c r="G21" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H21" s="10">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I21" s="10">
         <v>5</v>
@@ -11350,7 +11228,9 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19:L21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11786,27 +11666,27 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="83" t="s">
+      <c r="A19" s="85" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="9">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E19" s="61"/>
       <c r="F19" s="61">
         <v>30</v>
       </c>
       <c r="G19" s="10">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H19" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I19" s="10">
         <v>1</v>
@@ -11818,29 +11698,29 @@
         <v>105</v>
       </c>
       <c r="L19" s="55">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="86"/>
       <c r="B20" s="8">
         <v>7</v>
       </c>
       <c r="C20" s="9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D20" s="9">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E20" s="61"/>
       <c r="F20" s="61">
         <v>30</v>
       </c>
       <c r="G20" s="10">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H20" s="10">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="I20" s="10">
         <v>7</v>
@@ -11852,29 +11732,29 @@
         <v>106</v>
       </c>
       <c r="L20" s="55">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
       <c r="C21" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D21" s="9">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E21" s="61"/>
       <c r="F21" s="61">
         <v>30</v>
       </c>
       <c r="G21" s="10">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H21" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I21" s="10">
         <v>5</v>
@@ -11886,7 +11766,7 @@
         <v>107</v>
       </c>
       <c r="L21" s="55">
-        <v>360</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -12387,7 +12267,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12821,27 +12701,27 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="83" t="s">
+      <c r="A19" s="85" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E19" s="61"/>
       <c r="F19" s="61">
         <v>30</v>
       </c>
       <c r="G19" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H19" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I19" s="10">
         <v>1</v>
@@ -12857,25 +12737,25 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
+      <c r="A20" s="86"/>
       <c r="B20" s="8">
         <v>7</v>
       </c>
       <c r="C20" s="9">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D20" s="9">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E20" s="61"/>
       <c r="F20" s="61">
         <v>30</v>
       </c>
       <c r="G20" s="10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H20" s="10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I20" s="10">
         <v>7</v>
@@ -12891,25 +12771,25 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
       <c r="C21" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D21" s="9">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E21" s="61"/>
       <c r="F21" s="61">
         <v>30</v>
       </c>
       <c r="G21" s="10">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H21" s="10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I21" s="10">
         <v>5</v>

</xml_diff>

<commit_message>
Updates before Tallaght meeting
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="6996" tabRatio="843" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="6996" tabRatio="843" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="34" r:id="rId1"/>
@@ -1154,16 +1154,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1597,14 +1597,14 @@
       <c r="T1" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="83" t="s">
+      <c r="U1" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="84"/>
-      <c r="W1" s="85" t="s">
+      <c r="V1" s="86"/>
+      <c r="W1" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="86"/>
+      <c r="X1" s="84"/>
       <c r="Y1" s="87" t="s">
         <v>72</v>
       </c>
@@ -1612,10 +1612,10 @@
       <c r="AA1" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="85" t="s">
+      <c r="AB1" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="86"/>
+      <c r="AC1" s="84"/>
       <c r="AD1" t="s">
         <v>153</v>
       </c>
@@ -2272,14 +2272,14 @@
       <c r="T10" s="68">
         <v>0.28274342377083045</v>
       </c>
-      <c r="U10" s="83" t="s">
+      <c r="U10" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V10" s="84"/>
-      <c r="W10" s="85" t="s">
+      <c r="V10" s="86"/>
+      <c r="W10" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X10" s="86"/>
+      <c r="X10" s="84"/>
       <c r="Y10" s="87" t="s">
         <v>72</v>
       </c>
@@ -2287,10 +2287,10 @@
       <c r="AA10" t="s">
         <v>122</v>
       </c>
-      <c r="AB10" s="85" t="s">
+      <c r="AB10" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC10" s="86"/>
+      <c r="AC10" s="84"/>
       <c r="AD10" t="s">
         <v>153</v>
       </c>
@@ -2879,14 +2879,14 @@
       <c r="T18" s="68">
         <v>8.8705989940557842E-3</v>
       </c>
-      <c r="U18" s="83" t="s">
+      <c r="U18" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V18" s="84"/>
-      <c r="W18" s="85" t="s">
+      <c r="V18" s="86"/>
+      <c r="W18" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X18" s="86"/>
+      <c r="X18" s="84"/>
       <c r="Y18" s="87" t="s">
         <v>72</v>
       </c>
@@ -2894,10 +2894,10 @@
       <c r="AA18" t="s">
         <v>122</v>
       </c>
-      <c r="AB18" s="85" t="s">
+      <c r="AB18" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC18" s="86"/>
+      <c r="AC18" s="84"/>
       <c r="AD18" t="s">
         <v>153</v>
       </c>
@@ -3486,14 +3486,14 @@
       <c r="T26" s="68">
         <v>9.1654827918060579E-5</v>
       </c>
-      <c r="U26" s="83" t="s">
+      <c r="U26" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V26" s="84"/>
-      <c r="W26" s="85" t="s">
+      <c r="V26" s="86"/>
+      <c r="W26" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X26" s="86"/>
+      <c r="X26" s="84"/>
       <c r="Y26" s="87" t="s">
         <v>72</v>
       </c>
@@ -3501,10 +3501,10 @@
       <c r="AA26" t="s">
         <v>122</v>
       </c>
-      <c r="AB26" s="85" t="s">
+      <c r="AB26" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC26" s="86"/>
+      <c r="AC26" s="84"/>
       <c r="AD26" t="s">
         <v>153</v>
       </c>
@@ -4093,14 +4093,14 @@
       <c r="T34" s="68">
         <v>1.6580775263275824E-3</v>
       </c>
-      <c r="U34" s="83" t="s">
+      <c r="U34" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V34" s="84"/>
-      <c r="W34" s="85" t="s">
+      <c r="V34" s="86"/>
+      <c r="W34" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X34" s="86"/>
+      <c r="X34" s="84"/>
       <c r="Y34" s="87" t="s">
         <v>72</v>
       </c>
@@ -4108,10 +4108,10 @@
       <c r="AA34" t="s">
         <v>122</v>
       </c>
-      <c r="AB34" s="85" t="s">
+      <c r="AB34" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC34" s="86"/>
+      <c r="AC34" s="84"/>
       <c r="AD34" t="s">
         <v>153</v>
       </c>
@@ -4700,14 +4700,14 @@
       <c r="T42" s="68">
         <v>4.8399581113691206E-2</v>
       </c>
-      <c r="U42" s="83" t="s">
+      <c r="U42" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V42" s="84"/>
-      <c r="W42" s="85" t="s">
+      <c r="V42" s="86"/>
+      <c r="W42" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X42" s="86"/>
+      <c r="X42" s="84"/>
       <c r="Y42" s="87" t="s">
         <v>72</v>
       </c>
@@ -4715,10 +4715,10 @@
       <c r="AA42" t="s">
         <v>122</v>
       </c>
-      <c r="AB42" s="85" t="s">
+      <c r="AB42" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC42" s="86"/>
+      <c r="AC42" s="84"/>
       <c r="AD42" t="s">
         <v>153</v>
       </c>
@@ -5307,14 +5307,14 @@
       <c r="T50" s="68">
         <v>3.4685745335989858E-2</v>
       </c>
-      <c r="U50" s="83" t="s">
+      <c r="U50" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V50" s="84"/>
-      <c r="W50" s="85" t="s">
+      <c r="V50" s="86"/>
+      <c r="W50" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X50" s="86"/>
+      <c r="X50" s="84"/>
       <c r="Y50" s="87" t="s">
         <v>72</v>
       </c>
@@ -5322,10 +5322,10 @@
       <c r="AA50" t="s">
         <v>122</v>
       </c>
-      <c r="AB50" s="85" t="s">
+      <c r="AB50" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC50" s="86"/>
+      <c r="AC50" s="84"/>
       <c r="AD50" t="s">
         <v>153</v>
       </c>
@@ -5914,14 +5914,14 @@
       <c r="T58" s="68">
         <v>4.0882926165979244E-2</v>
       </c>
-      <c r="U58" s="83" t="s">
+      <c r="U58" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V58" s="84"/>
-      <c r="W58" s="85" t="s">
+      <c r="V58" s="86"/>
+      <c r="W58" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X58" s="86"/>
+      <c r="X58" s="84"/>
       <c r="Y58" s="87" t="s">
         <v>72</v>
       </c>
@@ -5929,10 +5929,10 @@
       <c r="AA58" t="s">
         <v>122</v>
       </c>
-      <c r="AB58" s="85" t="s">
+      <c r="AB58" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC58" s="86"/>
+      <c r="AC58" s="84"/>
       <c r="AD58" t="s">
         <v>153</v>
       </c>
@@ -6462,6 +6462,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="AB42:AC42"/>
     <mergeCell ref="AB50:AC50"/>
     <mergeCell ref="U58:V58"/>
     <mergeCell ref="W58:X58"/>
@@ -6470,30 +6494,6 @@
     <mergeCell ref="U50:V50"/>
     <mergeCell ref="W50:X50"/>
     <mergeCell ref="Y50:Z50"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="AB42:AC42"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AB10:AC10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8601,10 +8601,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8617,16 +8617,16 @@
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="85" t="s">
         <v>151</v>
       </c>
       <c r="C1" s="94"/>
-      <c r="D1" s="84"/>
-      <c r="J1" s="83" t="s">
+      <c r="D1" s="86"/>
+      <c r="J1" s="85" t="s">
         <v>152</v>
       </c>
       <c r="K1" s="94"/>
-      <c r="L1" s="84"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
@@ -8761,13 +8761,13 @@
         <v>59</v>
       </c>
       <c r="B9" s="30">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="C9" s="30">
         <v>60</v>
       </c>
       <c r="D9" s="30">
-        <v>720</v>
+        <v>420</v>
       </c>
       <c r="F9" s="30">
         <v>1140</v>
@@ -8875,6 +8875,32 @@
       </c>
       <c r="D13" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>B9/60</f>
+        <v>4.5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="0">C9/60</f>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>7*60</f>
+        <v>420</v>
+      </c>
+      <c r="J15">
+        <f>J9/60</f>
+        <v>1.5</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ref="K15:L15" si="1">K9/60</f>
+        <v>0.5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8908,11 +8934,11 @@
       <c r="A1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="85" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="94"/>
-      <c r="D1" s="84"/>
+      <c r="D1" s="86"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -10325,11 +10351,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD6" sqref="AD6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10422,14 +10448,14 @@
       <c r="T1" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="83" t="s">
+      <c r="U1" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="84"/>
-      <c r="W1" s="85" t="s">
+      <c r="V1" s="86"/>
+      <c r="W1" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="86"/>
+      <c r="X1" s="84"/>
       <c r="Y1" s="87" t="s">
         <v>72</v>
       </c>
@@ -10437,10 +10463,10 @@
       <c r="AA1" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="85" t="s">
+      <c r="AB1" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="86"/>
+      <c r="AC1" s="84"/>
       <c r="AD1" t="s">
         <v>153</v>
       </c>
@@ -10945,14 +10971,14 @@
       <c r="T10" s="68">
         <v>0.28274342377083045</v>
       </c>
-      <c r="U10" s="83" t="s">
+      <c r="U10" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V10" s="84"/>
-      <c r="W10" s="85" t="s">
+      <c r="V10" s="86"/>
+      <c r="W10" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X10" s="86"/>
+      <c r="X10" s="84"/>
       <c r="Y10" s="87" t="s">
         <v>72</v>
       </c>
@@ -10960,10 +10986,10 @@
       <c r="AA10" t="s">
         <v>122</v>
       </c>
-      <c r="AB10" s="85" t="s">
+      <c r="AB10" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC10" s="86"/>
+      <c r="AC10" s="84"/>
       <c r="AD10" t="s">
         <v>153</v>
       </c>
@@ -11552,14 +11578,14 @@
       <c r="T18" s="68">
         <v>8.8705989940557842E-3</v>
       </c>
-      <c r="U18" s="83" t="s">
+      <c r="U18" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V18" s="84"/>
-      <c r="W18" s="85" t="s">
+      <c r="V18" s="86"/>
+      <c r="W18" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X18" s="86"/>
+      <c r="X18" s="84"/>
       <c r="Y18" s="87" t="s">
         <v>72</v>
       </c>
@@ -11567,10 +11593,10 @@
       <c r="AA18" t="s">
         <v>122</v>
       </c>
-      <c r="AB18" s="85" t="s">
+      <c r="AB18" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC18" s="86"/>
+      <c r="AC18" s="84"/>
       <c r="AD18" t="s">
         <v>153</v>
       </c>
@@ -12159,14 +12185,14 @@
       <c r="T26" s="68">
         <v>9.1654827918060579E-5</v>
       </c>
-      <c r="U26" s="83" t="s">
+      <c r="U26" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V26" s="84"/>
-      <c r="W26" s="85" t="s">
+      <c r="V26" s="86"/>
+      <c r="W26" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X26" s="86"/>
+      <c r="X26" s="84"/>
       <c r="Y26" s="87" t="s">
         <v>72</v>
       </c>
@@ -12174,10 +12200,10 @@
       <c r="AA26" t="s">
         <v>122</v>
       </c>
-      <c r="AB26" s="85" t="s">
+      <c r="AB26" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC26" s="86"/>
+      <c r="AC26" s="84"/>
       <c r="AD26" t="s">
         <v>153</v>
       </c>
@@ -12766,14 +12792,14 @@
       <c r="T34" s="68">
         <v>1.6580775263275824E-3</v>
       </c>
-      <c r="U34" s="83" t="s">
+      <c r="U34" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V34" s="84"/>
-      <c r="W34" s="85" t="s">
+      <c r="V34" s="86"/>
+      <c r="W34" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X34" s="86"/>
+      <c r="X34" s="84"/>
       <c r="Y34" s="87" t="s">
         <v>72</v>
       </c>
@@ -12781,10 +12807,10 @@
       <c r="AA34" t="s">
         <v>122</v>
       </c>
-      <c r="AB34" s="85" t="s">
+      <c r="AB34" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC34" s="86"/>
+      <c r="AC34" s="84"/>
       <c r="AD34" t="s">
         <v>153</v>
       </c>
@@ -13373,14 +13399,14 @@
       <c r="T42" s="68">
         <v>4.8399581113691206E-2</v>
       </c>
-      <c r="U42" s="83" t="s">
+      <c r="U42" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V42" s="84"/>
-      <c r="W42" s="85" t="s">
+      <c r="V42" s="86"/>
+      <c r="W42" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X42" s="86"/>
+      <c r="X42" s="84"/>
       <c r="Y42" s="87" t="s">
         <v>72</v>
       </c>
@@ -13388,10 +13414,10 @@
       <c r="AA42" t="s">
         <v>122</v>
       </c>
-      <c r="AB42" s="85" t="s">
+      <c r="AB42" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC42" s="86"/>
+      <c r="AC42" s="84"/>
       <c r="AD42" t="s">
         <v>153</v>
       </c>
@@ -13980,14 +14006,14 @@
       <c r="T50" s="68">
         <v>3.4685745335989858E-2</v>
       </c>
-      <c r="U50" s="83" t="s">
+      <c r="U50" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V50" s="84"/>
-      <c r="W50" s="85" t="s">
+      <c r="V50" s="86"/>
+      <c r="W50" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X50" s="86"/>
+      <c r="X50" s="84"/>
       <c r="Y50" s="87" t="s">
         <v>72</v>
       </c>
@@ -13995,10 +14021,10 @@
       <c r="AA50" t="s">
         <v>122</v>
       </c>
-      <c r="AB50" s="85" t="s">
+      <c r="AB50" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC50" s="86"/>
+      <c r="AC50" s="84"/>
       <c r="AD50" t="s">
         <v>153</v>
       </c>
@@ -14587,14 +14613,14 @@
       <c r="T58" s="68">
         <v>4.0882926165979244E-2</v>
       </c>
-      <c r="U58" s="83" t="s">
+      <c r="U58" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="V58" s="84"/>
-      <c r="W58" s="85" t="s">
+      <c r="V58" s="86"/>
+      <c r="W58" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="X58" s="86"/>
+      <c r="X58" s="84"/>
       <c r="Y58" s="87" t="s">
         <v>72</v>
       </c>
@@ -14602,10 +14628,10 @@
       <c r="AA58" t="s">
         <v>122</v>
       </c>
-      <c r="AB58" s="85" t="s">
+      <c r="AB58" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="AC58" s="86"/>
+      <c r="AC58" s="84"/>
       <c r="AD58" t="s">
         <v>153</v>
       </c>
@@ -15135,6 +15161,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="Y42:Z42"/>
+    <mergeCell ref="AB42:AC42"/>
     <mergeCell ref="U50:V50"/>
     <mergeCell ref="W50:X50"/>
     <mergeCell ref="Y50:Z50"/>
@@ -15143,30 +15193,6 @@
     <mergeCell ref="W58:X58"/>
     <mergeCell ref="Y58:Z58"/>
     <mergeCell ref="AB58:AC58"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="Y42:Z42"/>
-    <mergeCell ref="AB42:AC42"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AB10:AC10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19391,7 +19417,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19471,7 +19497,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="25">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -19515,7 +19541,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="25">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -20121,8 +20147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J1" sqref="B1:J1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20140,31 +20166,31 @@
   <sheetData>
     <row r="1" spans="2:10" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>8.6709188687995447</v>
+        <v>6.9656026932429755</v>
       </c>
       <c r="C1" s="68">
-        <v>19.484876308368534</v>
+        <v>12.677415235839224</v>
       </c>
       <c r="D1" s="68">
-        <v>5.8261029550789702</v>
+        <v>5.3916514362385959</v>
       </c>
       <c r="E1" s="68">
-        <v>11.043840613928195</v>
+        <v>8.86963223299772</v>
       </c>
       <c r="F1" s="68">
-        <v>19.414492273627449</v>
+        <v>13.181824797489693</v>
       </c>
       <c r="G1" s="68">
-        <v>7.859760740816597</v>
+        <v>7.2209819428035225</v>
       </c>
       <c r="H1" s="68">
-        <v>4.1238951066963621</v>
+        <v>4.8250184007989478</v>
       </c>
       <c r="I1" s="68">
-        <v>4.7478920483373726</v>
+        <v>5.8061926198639195</v>
       </c>
       <c r="J1" s="68">
-        <v>3.4982222556328595</v>
+        <v>3.8330915875524409</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
@@ -20381,39 +20407,39 @@
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>6.5933174863420811</v>
+        <v>6.3090981237493189</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>13.435959661066709</v>
+        <v>12.301382815645157</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>4.5388589920079365</v>
+        <v>4.4664504055345402</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>8.1339152979384348</v>
+        <v>7.771547234450022</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>13.901938127249439</v>
+        <v>12.863160214559812</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>5.8173689831612663</v>
+        <v>5.7109058501590866</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>4.1129724157691099</v>
+        <v>4.2298262981195416</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>4.8525824989999862</v>
+        <v>5.0289659275877447</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>3.3860440218474763</v>
+        <v>3.4418555771674058</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -20448,39 +20474,39 @@
     <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="76">
         <f t="shared" ref="B17:D17" si="1">B1-B18</f>
-        <v>8.6709188687995447</v>
+        <v>6.9656026932429755</v>
       </c>
       <c r="C17" s="76">
         <f t="shared" si="1"/>
-        <v>19.484876308368534</v>
+        <v>12.677415235839224</v>
       </c>
       <c r="D17" s="76">
         <f t="shared" si="1"/>
-        <v>5.8261029550789702</v>
+        <v>5.3916514362385959</v>
       </c>
       <c r="E17" s="76">
-        <f t="shared" ref="E17:J17" si="2">E13-E18</f>
-        <v>-2.2760847020615653</v>
+        <f>E1-E18</f>
+        <v>-1.5403677670022802</v>
       </c>
       <c r="F17" s="76">
-        <f t="shared" si="2"/>
-        <v>-2.4580618727505605</v>
+        <f t="shared" ref="F17" si="2">F1-F18</f>
+        <v>-3.1781752025103067</v>
       </c>
       <c r="G17" s="76">
-        <f t="shared" si="2"/>
-        <v>-0.90263101683873348</v>
+        <f t="shared" ref="G17" si="3">G1-G18</f>
+        <v>0.50098194280352271</v>
       </c>
       <c r="H17" s="76">
-        <f t="shared" si="2"/>
-        <v>-0.34702758423089008</v>
+        <f t="shared" ref="H17:I17" si="4">H1-H18</f>
+        <v>0.36501840079894787</v>
       </c>
       <c r="I17" s="76">
-        <f t="shared" si="2"/>
-        <v>3.2582498999985887E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.98619261986391926</v>
       </c>
       <c r="J17" s="76">
-        <f t="shared" si="2"/>
-        <v>-0.70395597815252353</v>
+        <f t="shared" ref="J17" si="5">J1-J18</f>
+        <v>-0.25690841244755891</v>
       </c>
       <c r="K17" s="75"/>
       <c r="L17" s="75"/>
@@ -20571,34 +20597,34 @@
   <sheetData>
     <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>9.848342971193885</v>
+        <v>8.1551240098546582</v>
       </c>
       <c r="C1" s="68">
-        <v>20.557192854610278</v>
+        <v>13.825038536601168</v>
       </c>
       <c r="D1" s="68">
-        <v>7.0311775868992861</v>
+        <v>6.592718200853108</v>
       </c>
       <c r="E1" s="68">
-        <v>45.355191256830601</v>
+        <v>48.989841342312523</v>
       </c>
       <c r="F1" s="68">
-        <v>52.196699375557543</v>
+        <v>60.111846610362932</v>
       </c>
       <c r="G1" s="68">
-        <v>57.112676056338032</v>
+        <v>60.60561944970155</v>
       </c>
       <c r="H1" s="68">
-        <v>64.821856076608924</v>
+        <v>70.043668122270745</v>
       </c>
       <c r="I1" s="68">
-        <v>0.88890399782431329</v>
+        <v>0.91221496138555047</v>
       </c>
       <c r="J1" s="68">
-        <v>0.25482730486809901</v>
+        <v>0.25595210894301512</v>
       </c>
       <c r="K1" s="68">
-        <v>9.2738645635028552E-2</v>
+        <v>6.6352876662249233E-2</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
@@ -20836,43 +20862,43 @@
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>7.60903396473583</v>
+        <v>7.3268308045126256</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>14.379522192940227</v>
+        <v>13.257496473272042</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>5.563677201717776</v>
+        <v>5.4906006373767449</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>60.263926556052667</v>
+        <v>60.869701570299661</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>67.364028413460048</v>
+        <v>68.683219619260953</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>72.048982823179117</v>
+        <v>72.631140055406362</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>78.832925358204008</v>
+        <v>79.7032273658143</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.85369893178645551</v>
+        <v>0.857584092379995</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.21996148503530777</v>
+        <v>0.22014895238112711</v>
       </c>
       <c r="K13" s="67">
         <f>AVERAGE(K1:K10)</f>
-        <v>4.225355803713262E-2</v>
+        <v>3.7855929875002733E-2</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -21010,14 +21036,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="85" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="86"/>
+      <c r="D1" s="84"/>
       <c r="E1" s="87" t="s">
         <v>72</v>
       </c>
@@ -21031,23 +21057,23 @@
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16666285444162302</v>
+        <v>0.16666281995060775</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>0.2838533941313196</v>
+        <v>0.29253529162397246</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>590.90057827163309</v>
+        <v>489.30744059127954</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>0.41034762379974521</v>
+        <v>0.33979683374394415</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -21061,13 +21087,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.24123441659296949</v>
+        <v>0.29438058499999303</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>45.334968230966446</v>
+        <v>49.013120365088419</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -21075,19 +21101,19 @@
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>17.714968152866245</v>
+        <v>18.096723868954761</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>6.9993284910077447E-2</v>
+        <v>7.3169490587602928E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>52.173428444048156</v>
+        <v>60.130047912388775</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -21095,19 +21121,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>83.440063366762089</v>
+        <v>80.115392214977149</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>52.729646069752746</v>
+        <v>62.380194111969075</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.1371694067190816</v>
+        <v>7.4741019214703268</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -21115,23 +21141,23 @@
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>30.373476268695303</v>
+        <v>32.482584976919767</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.18010325244752148</v>
+        <v>0.17803059826723192</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>-1479.3985434368899</v>
+        <v>-1697.1896070057064</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>-1.0273600996089514</v>
+        <v>-1.1786038937539627</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -21139,13 +21165,13 @@
         <v>103</v>
       </c>
       <c r="B7" s="38">
-        <v>34.881164776347681</v>
+        <v>33.865012792693591</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.30004198747946687</v>
+        <v>0.31772214505537399</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -21163,17 +21189,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>0.32211690003161708</v>
+        <v>0.33383836588636501</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>6.1200827445291442E-2</v>
+        <v>8.5943355172068331E-2</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>4.2500574614785722E-5</v>
+        <v>5.9682885536158564E-5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -21185,17 +21211,17 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="84"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="36">
-        <v>0.11330279348988682</v>
+        <v>0.11510178259569369</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -21203,7 +21229,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="36">
-        <v>0.25433517167270925</v>
+        <v>0.2534053163955719</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -21219,7 +21245,7 @@
         <v>70</v>
       </c>
       <c r="D16" s="36">
-        <v>31.86725764754523</v>
+        <v>33.512273687959706</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
@@ -21235,7 +21261,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="36">
-        <v>5.4888926407057947E-2</v>
+        <v>5.7217923541754721E-2</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
@@ -21243,7 +21269,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="36">
-        <v>4.6746002864793294E-2</v>
+        <v>6.4018006548187387E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes after Tallaght presentation
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model/control.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="6996" tabRatio="843" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="6996" tabRatio="843" firstSheet="2" activeTab="18"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="34" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="35" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="34" state="hidden" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="35" state="hidden" r:id="rId2"/>
     <sheet name="Sim Runs (2)" sheetId="33" r:id="rId3"/>
     <sheet name="Sim Runs" sheetId="29" r:id="rId4"/>
     <sheet name="Output" sheetId="27" r:id="rId5"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="159">
   <si>
     <t>Resources/Process</t>
   </si>
@@ -547,6 +547,12 @@
   </si>
   <si>
     <t>1'</t>
+  </si>
+  <si>
+    <t>Amb_2_Med_Non</t>
+  </si>
+  <si>
+    <t>WI_2_Med_Non</t>
   </si>
 </sst>
 </file>
@@ -1501,31 +1507,31 @@
   <dimension ref="A1:AD65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="W47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC38" sqref="AC38"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.21875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="19.88671875" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="14.33203125" hidden="1" customWidth="1"/>
-    <col min="16" max="17" width="25.109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+    <col min="14" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="17" width="25.109375" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" customWidth="1"/>
     <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
@@ -8604,7 +8610,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8879,27 +8885,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15">
-        <f>B9/60</f>
-        <v>4.5</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:D15" si="0">C9/60</f>
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <f>7*60</f>
-        <v>420</v>
+        <f>4.5*60</f>
+        <v>270</v>
       </c>
       <c r="J15">
         <f>J9/60</f>
         <v>1.5</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:L15" si="1">K9/60</f>
+        <f t="shared" ref="K15:L15" si="0">K9/60</f>
         <v>0.5</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -9930,9 +9928,11 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9943,9 +9943,13 @@
     <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
@@ -9966,9 +9970,20 @@
       <c r="H1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="28"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -9989,17 +10004,26 @@
       <c r="H2" s="24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>0</v>
       </c>
       <c r="B3" s="25">
         <v>1.25</v>
       </c>
-      <c r="C3">
-        <v>25</v>
-      </c>
       <c r="D3" s="22">
         <v>0</v>
       </c>
@@ -10015,17 +10039,26 @@
       <c r="I3" s="31" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3" s="22">
+        <v>0</v>
+      </c>
+      <c r="K3" s="25">
+        <v>58</v>
+      </c>
+      <c r="M3" s="22">
+        <v>0</v>
+      </c>
+      <c r="N3" s="25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
       <c r="B4" s="25">
         <v>98.75</v>
       </c>
-      <c r="C4">
-        <v>75</v>
-      </c>
       <c r="D4" s="22">
         <v>1</v>
       </c>
@@ -10041,8 +10074,20 @@
       <c r="I4" s="31" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" s="22">
+        <v>1</v>
+      </c>
+      <c r="K4" s="25">
+        <v>42</v>
+      </c>
+      <c r="M4" s="22">
+        <v>1</v>
+      </c>
+      <c r="N4" s="25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -10060,8 +10105,16 @@
       <c r="I5" s="31" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" s="22">
+        <v>2</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="M5" s="22">
+        <v>2</v>
+      </c>
+      <c r="N5" s="25"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -10079,8 +10132,16 @@
       <c r="I6" s="31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" s="22">
+        <v>3</v>
+      </c>
+      <c r="K6" s="25"/>
+      <c r="M6" s="22">
+        <v>3</v>
+      </c>
+      <c r="N6" s="25"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -10093,8 +10154,16 @@
         <v>4</v>
       </c>
       <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7" s="22">
+        <v>4</v>
+      </c>
+      <c r="K7" s="25"/>
+      <c r="M7" s="22">
+        <v>4</v>
+      </c>
+      <c r="N7" s="25"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -10107,8 +10176,16 @@
         <v>5</v>
       </c>
       <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" s="22">
+        <v>5</v>
+      </c>
+      <c r="K8" s="25"/>
+      <c r="M8" s="22">
+        <v>5</v>
+      </c>
+      <c r="N8" s="25"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -10121,8 +10198,16 @@
         <v>6</v>
       </c>
       <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="22">
+        <v>6</v>
+      </c>
+      <c r="K9" s="25"/>
+      <c r="M9" s="22">
+        <v>6</v>
+      </c>
+      <c r="N9" s="25"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -10135,8 +10220,16 @@
         <v>7</v>
       </c>
       <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" s="22">
+        <v>7</v>
+      </c>
+      <c r="K10" s="25"/>
+      <c r="M10" s="22">
+        <v>7</v>
+      </c>
+      <c r="N10" s="25"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -10149,8 +10242,16 @@
         <v>8</v>
       </c>
       <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11" s="22">
+        <v>8</v>
+      </c>
+      <c r="K11" s="25"/>
+      <c r="M11" s="22">
+        <v>8</v>
+      </c>
+      <c r="N11" s="25"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -10163,8 +10264,16 @@
         <v>9</v>
       </c>
       <c r="H12" s="25"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="22">
+        <v>9</v>
+      </c>
+      <c r="K12" s="25"/>
+      <c r="M12" s="22">
+        <v>9</v>
+      </c>
+      <c r="N12" s="25"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -10177,8 +10286,16 @@
         <v>10</v>
       </c>
       <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="22">
+        <v>10</v>
+      </c>
+      <c r="K13" s="25"/>
+      <c r="M13" s="22">
+        <v>10</v>
+      </c>
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -10191,8 +10308,16 @@
         <v>11</v>
       </c>
       <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J14" s="22">
+        <v>11</v>
+      </c>
+      <c r="K14" s="25"/>
+      <c r="M14" s="22">
+        <v>11</v>
+      </c>
+      <c r="N14" s="25"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -10205,8 +10330,16 @@
         <v>12</v>
       </c>
       <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J15" s="22">
+        <v>12</v>
+      </c>
+      <c r="K15" s="25"/>
+      <c r="M15" s="22">
+        <v>12</v>
+      </c>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -10219,8 +10352,16 @@
         <v>13</v>
       </c>
       <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J16" s="22">
+        <v>13</v>
+      </c>
+      <c r="K16" s="25"/>
+      <c r="M16" s="22">
+        <v>13</v>
+      </c>
+      <c r="N16" s="25"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -10233,8 +10374,16 @@
         <v>14</v>
       </c>
       <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J17" s="22">
+        <v>14</v>
+      </c>
+      <c r="K17" s="25"/>
+      <c r="M17" s="22">
+        <v>14</v>
+      </c>
+      <c r="N17" s="25"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -10247,8 +10396,16 @@
         <v>15</v>
       </c>
       <c r="H18" s="25"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J18" s="22">
+        <v>15</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="M18" s="22">
+        <v>15</v>
+      </c>
+      <c r="N18" s="25"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>16</v>
       </c>
@@ -10261,8 +10418,16 @@
         <v>16</v>
       </c>
       <c r="H19" s="25"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J19" s="22">
+        <v>16</v>
+      </c>
+      <c r="K19" s="25"/>
+      <c r="M19" s="22">
+        <v>16</v>
+      </c>
+      <c r="N19" s="25"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>17</v>
       </c>
@@ -10275,8 +10440,16 @@
         <v>17</v>
       </c>
       <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J20" s="22">
+        <v>17</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="M20" s="22">
+        <v>17</v>
+      </c>
+      <c r="N20" s="25"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>18</v>
       </c>
@@ -10289,8 +10462,16 @@
         <v>18</v>
       </c>
       <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J21" s="22">
+        <v>18</v>
+      </c>
+      <c r="K21" s="25"/>
+      <c r="M21" s="22">
+        <v>18</v>
+      </c>
+      <c r="N21" s="25"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>19</v>
       </c>
@@ -10303,8 +10484,16 @@
         <v>19</v>
       </c>
       <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J22" s="22">
+        <v>19</v>
+      </c>
+      <c r="K22" s="25"/>
+      <c r="M22" s="22">
+        <v>19</v>
+      </c>
+      <c r="N22" s="25"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>20</v>
       </c>
@@ -10317,8 +10506,16 @@
         <v>20</v>
       </c>
       <c r="H23" s="25"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J23" s="22">
+        <v>20</v>
+      </c>
+      <c r="K23" s="25"/>
+      <c r="M23" s="22">
+        <v>20</v>
+      </c>
+      <c r="N23" s="25"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -10338,6 +10535,20 @@
       </c>
       <c r="H24" s="27">
         <f>SUM(H3:H23)</f>
+        <v>100</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="27">
+        <f>SUM(K3:K23)</f>
+        <v>100</v>
+      </c>
+      <c r="M24" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" s="27">
+        <f>SUM(N3:N23)</f>
         <v>100</v>
       </c>
     </row>
@@ -20147,7 +20358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -20166,31 +20377,31 @@
   <sheetData>
     <row r="1" spans="2:10" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>6.9656026932429755</v>
+        <v>7.418019809509504</v>
       </c>
       <c r="C1" s="68">
-        <v>12.677415235839224</v>
+        <v>13.511937243566711</v>
       </c>
       <c r="D1" s="68">
-        <v>5.3916514362385959</v>
+        <v>5.7501925209076754</v>
       </c>
       <c r="E1" s="68">
-        <v>8.86963223299772</v>
+        <v>9.2676527199407879</v>
       </c>
       <c r="F1" s="68">
-        <v>13.181824797489693</v>
+        <v>13.95790490930232</v>
       </c>
       <c r="G1" s="68">
-        <v>7.2209819428035225</v>
+        <v>7.4933465920283995</v>
       </c>
       <c r="H1" s="68">
-        <v>4.8250184007989478</v>
+        <v>4.8103271344292358</v>
       </c>
       <c r="I1" s="68">
-        <v>5.8061926198639195</v>
+        <v>5.8730845359241481</v>
       </c>
       <c r="J1" s="68">
-        <v>3.8330915875524409</v>
+        <v>3.7233703234126363</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
@@ -20407,39 +20618,39 @@
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>6.3090981237493189</v>
+        <v>6.3845009764604077</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>12.301382815645157</v>
+        <v>12.440469816933073</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>4.4664504055345402</v>
+        <v>4.5262072529793871</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>7.771547234450022</v>
+        <v>7.8378839822738664</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>12.863160214559812</v>
+        <v>12.992506899861917</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>5.7109058501590866</v>
+        <v>5.7562999583632326</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>4.2298262981195416</v>
+        <v>4.2273777537245882</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>5.0289659275877447</v>
+        <v>5.0401145802644498</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>3.4418555771674058</v>
+        <v>3.4235686998107724</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -20474,39 +20685,39 @@
     <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="76">
         <f t="shared" ref="B17:D17" si="1">B1-B18</f>
-        <v>6.9656026932429755</v>
+        <v>7.418019809509504</v>
       </c>
       <c r="C17" s="76">
         <f t="shared" si="1"/>
-        <v>12.677415235839224</v>
+        <v>13.511937243566711</v>
       </c>
       <c r="D17" s="76">
         <f t="shared" si="1"/>
-        <v>5.3916514362385959</v>
+        <v>5.7501925209076754</v>
       </c>
       <c r="E17" s="76">
         <f>E1-E18</f>
-        <v>-1.5403677670022802</v>
+        <v>-1.1423472800592123</v>
       </c>
       <c r="F17" s="76">
         <f t="shared" ref="F17" si="2">F1-F18</f>
-        <v>-3.1781752025103067</v>
+        <v>-2.4020950906976797</v>
       </c>
       <c r="G17" s="76">
         <f t="shared" ref="G17" si="3">G1-G18</f>
-        <v>0.50098194280352271</v>
+        <v>0.77334659202839973</v>
       </c>
       <c r="H17" s="76">
         <f t="shared" ref="H17:I17" si="4">H1-H18</f>
-        <v>0.36501840079894787</v>
+        <v>0.3503271344292358</v>
       </c>
       <c r="I17" s="76">
         <f t="shared" si="4"/>
-        <v>0.98619261986391926</v>
+        <v>1.0530845359241479</v>
       </c>
       <c r="J17" s="76">
         <f t="shared" ref="J17" si="5">J1-J18</f>
-        <v>-0.25690841244755891</v>
+        <v>-0.36662967658736356</v>
       </c>
       <c r="K17" s="75"/>
       <c r="L17" s="75"/>
@@ -20597,34 +20808,34 @@
   <sheetData>
     <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>8.1551240098546582</v>
+        <v>8.6152683913188124</v>
       </c>
       <c r="C1" s="68">
-        <v>13.825038536601168</v>
+        <v>14.647847014632349</v>
       </c>
       <c r="D1" s="68">
-        <v>6.592718200853108</v>
+        <v>6.9642287509770489</v>
       </c>
       <c r="E1" s="68">
-        <v>48.989841342312523</v>
+        <v>46.634561541046033</v>
       </c>
       <c r="F1" s="68">
-        <v>60.111846610362932</v>
+        <v>56.651735722284435</v>
       </c>
       <c r="G1" s="68">
-        <v>60.60561944970155</v>
+        <v>58.279845956354301</v>
       </c>
       <c r="H1" s="68">
-        <v>70.043668122270745</v>
+        <v>67.099258414147172</v>
       </c>
       <c r="I1" s="68">
-        <v>0.91221496138555047</v>
+        <v>0.90045372050816697</v>
       </c>
       <c r="J1" s="68">
-        <v>0.25595210894301512</v>
+        <v>0.25503629764065333</v>
       </c>
       <c r="K1" s="68">
-        <v>6.6352876662249233E-2</v>
+        <v>7.994555353901997E-2</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
@@ -20862,43 +21073,43 @@
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>7.3268308045126256</v>
+        <v>7.4035215347566519</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>13.257496473272042</v>
+        <v>13.394631219610574</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>5.4906006373767449</v>
+        <v>5.5525190623974021</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>60.869701570299661</v>
+        <v>60.477154936755234</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>68.683219619260953</v>
+        <v>68.106534471247855</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>72.631140055406362</v>
+        <v>72.243511139848493</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>79.7032273658143</v>
+        <v>79.212492414460385</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.857584092379995</v>
+        <v>0.85562388556709779</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.22014895238112711</v>
+        <v>0.21999631716406678</v>
       </c>
       <c r="K13" s="67">
         <f>AVERAGE(K1:K10)</f>
-        <v>3.7855929875002733E-2</v>
+        <v>4.0121376021131187E-2</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -21021,7 +21232,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21057,23 +21268,23 @@
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16666281995060775</v>
+        <v>0.16666284640245677</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>0.29253529162397246</v>
+        <v>0.28550918862585356</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>489.30744059127954</v>
+        <v>516.91610347912876</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>0.33979683374394415</v>
+        <v>0.35896951630495055</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -21087,13 +21298,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.29438058499999303</v>
+        <v>0.24506931708508964</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>49.013120365088419</v>
+        <v>46.658457405127059</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -21101,19 +21312,19 @@
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>18.096723868954761</v>
+        <v>20.317220543806648</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>7.3169490587602928E-2</v>
+        <v>7.2407045121109945E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>60.130047912388775</v>
+        <v>56.671143944481749</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -21121,19 +21332,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>80.115392214977149</v>
+        <v>81.075396983061395</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>62.380194111969075</v>
+        <v>54.341704605894435</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.4741019214703268</v>
+        <v>7.1380279710450623</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -21141,23 +21352,23 @@
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>32.482584976919767</v>
+        <v>31.742575909242664</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.17803059826723192</v>
+        <v>0.17990907077693735</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>-1697.1896070057064</v>
+        <v>-1731.0923948154302</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>-1.1786038937539627</v>
+        <v>-1.2021474963996044</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -21165,13 +21376,13 @@
         <v>103</v>
       </c>
       <c r="B7" s="38">
-        <v>33.865012792693591</v>
+        <v>71.322733967063868</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.31772214505537399</v>
+        <v>0.30857998713522794</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -21189,17 +21400,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>0.33383836588636501</v>
+        <v>0.33001476609202235</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>8.5943355172068331E-2</v>
+        <v>6.8418880210536659E-2</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>5.9682885536158564E-5</v>
+        <v>4.7513111257317125E-5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -21221,7 +21432,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="36">
-        <v>0.11510178259569369</v>
+        <v>0.11298584127484131</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -21229,7 +21440,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="36">
-        <v>0.2534053163955719</v>
+        <v>0.24455768231903996</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -21245,7 +21456,7 @@
         <v>70</v>
       </c>
       <c r="D16" s="36">
-        <v>33.512273687959706</v>
+        <v>29.549979442023851</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
@@ -21261,7 +21472,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="36">
-        <v>5.7217923541754721E-2</v>
+        <v>5.3750426634411388E-2</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
@@ -21269,7 +21480,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="36">
-        <v>6.4018006548187387E-2</v>
+        <v>7.3121828077982023E-2</v>
       </c>
     </row>
   </sheetData>
@@ -21307,7 +21518,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>